<commit_message>
modelo inicial - trabalho 02
</commit_message>
<xml_diff>
--- a/trabalho02/rascunho.xlsx
+++ b/trabalho02/rascunho.xlsx
@@ -8,56 +8,159 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/acsjunior/Documents/Projects/ppgmne-mnum7078/trabalho02/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10FEA729-60A7-7F46-90D1-1E1EFBB6CFA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84E78CD0-27BB-2146-88D8-071A10E4B03F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16940" xr2:uid="{8808CF02-2367-564A-820C-A633E855AC6A}"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16940" activeTab="1" xr2:uid="{8808CF02-2367-564A-820C-A633E855AC6A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1 (2)" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet5" sheetId="5" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="solver_adj" localSheetId="0" hidden="1">Sheet1!$J$8:$M$11,Sheet1!$J$13:$M$16,Sheet1!#REF!,Sheet1!#REF!</definedName>
+    <definedName name="solver_adj" localSheetId="1" hidden="1">'Sheet1 (2)'!$P$8:$S$11,'Sheet1 (2)'!$P$17:$S$17,'Sheet1 (2)'!$P$20:$S$23,'Sheet1 (2)'!$P$35:$S$35,'Sheet1 (2)'!$P$41:$S$44,'Sheet1 (2)'!$P$50:$S$50,'Sheet1 (2)'!$P$53:$S$56,'Sheet1 (2)'!$P$68:$S$68</definedName>
+    <definedName name="solver_adj" localSheetId="4" hidden="1">Sheet2!$AJ$10:$AN$10</definedName>
     <definedName name="solver_cvg" localSheetId="0" hidden="1">0.0001</definedName>
+    <definedName name="solver_cvg" localSheetId="1" hidden="1">0.0001</definedName>
+    <definedName name="solver_cvg" localSheetId="4" hidden="1">0.0001</definedName>
     <definedName name="solver_drv" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_drv" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_drv" localSheetId="4" hidden="1">1</definedName>
     <definedName name="solver_eng" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_eng" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_eng" localSheetId="4" hidden="1">2</definedName>
     <definedName name="solver_itr" localSheetId="0" hidden="1">2147483647</definedName>
+    <definedName name="solver_itr" localSheetId="1" hidden="1">2147483647</definedName>
+    <definedName name="solver_itr" localSheetId="4" hidden="1">2147483647</definedName>
     <definedName name="solver_lhs1" localSheetId="0" hidden="1">Sheet1!$J$17:$M$17</definedName>
+    <definedName name="solver_lhs1" localSheetId="1" hidden="1">'Sheet1 (2)'!$P$14:$S$14</definedName>
+    <definedName name="solver_lhs1" localSheetId="4" hidden="1">Sheet2!$AO$12</definedName>
+    <definedName name="solver_lhs10" localSheetId="1" hidden="1">'Sheet1 (2)'!$P$65</definedName>
+    <definedName name="solver_lhs11" localSheetId="1" hidden="1">'Sheet1 (2)'!$P$68:$S$68</definedName>
+    <definedName name="solver_lhs12" localSheetId="1" hidden="1">'Sheet1 (2)'!$T$41:$T$44</definedName>
+    <definedName name="solver_lhs13" localSheetId="1" hidden="1">'Sheet1 (2)'!$T$8:$T$11</definedName>
     <definedName name="solver_lhs2" localSheetId="0" hidden="1">Sheet1!#REF!</definedName>
+    <definedName name="solver_lhs2" localSheetId="1" hidden="1">'Sheet1 (2)'!$P$17:$S$17</definedName>
+    <definedName name="solver_lhs2" localSheetId="4" hidden="1">Sheet2!$AO$13</definedName>
     <definedName name="solver_lhs3" localSheetId="0" hidden="1">Sheet1!#REF!</definedName>
+    <definedName name="solver_lhs3" localSheetId="1" hidden="1">'Sheet1 (2)'!$P$17:$S$17</definedName>
+    <definedName name="solver_lhs3" localSheetId="4" hidden="1">Sheet2!$AO$14</definedName>
     <definedName name="solver_lhs4" localSheetId="0" hidden="1">Sheet1!$N$8:$N$11</definedName>
+    <definedName name="solver_lhs4" localSheetId="1" hidden="1">'Sheet1 (2)'!$P$32</definedName>
     <definedName name="solver_lhs5" localSheetId="0" hidden="1">Sheet1!#REF!</definedName>
+    <definedName name="solver_lhs5" localSheetId="1" hidden="1">'Sheet1 (2)'!$P$35:$S$35</definedName>
+    <definedName name="solver_lhs6" localSheetId="1" hidden="1">'Sheet1 (2)'!$P$36</definedName>
+    <definedName name="solver_lhs7" localSheetId="1" hidden="1">'Sheet1 (2)'!$P$47:$S$47</definedName>
+    <definedName name="solver_lhs8" localSheetId="1" hidden="1">'Sheet1 (2)'!$P$50:$S$50</definedName>
+    <definedName name="solver_lhs9" localSheetId="1" hidden="1">'Sheet1 (2)'!$P$50:$S$50</definedName>
     <definedName name="solver_lin" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_lin" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_lin" localSheetId="4" hidden="1">1</definedName>
     <definedName name="solver_mip" localSheetId="0" hidden="1">2147483647</definedName>
+    <definedName name="solver_mip" localSheetId="1" hidden="1">2147483647</definedName>
+    <definedName name="solver_mip" localSheetId="4" hidden="1">2147483647</definedName>
     <definedName name="solver_mni" localSheetId="0" hidden="1">30</definedName>
+    <definedName name="solver_mni" localSheetId="1" hidden="1">30</definedName>
+    <definedName name="solver_mni" localSheetId="4" hidden="1">30</definedName>
     <definedName name="solver_mrt" localSheetId="0" hidden="1">0.075</definedName>
+    <definedName name="solver_mrt" localSheetId="1" hidden="1">0.075</definedName>
+    <definedName name="solver_mrt" localSheetId="4" hidden="1">0.075</definedName>
     <definedName name="solver_msl" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_msl" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_msl" localSheetId="4" hidden="1">2</definedName>
     <definedName name="solver_neg" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_neg" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_neg" localSheetId="4" hidden="1">1</definedName>
     <definedName name="solver_nod" localSheetId="0" hidden="1">2147483647</definedName>
+    <definedName name="solver_nod" localSheetId="1" hidden="1">2147483647</definedName>
+    <definedName name="solver_nod" localSheetId="4" hidden="1">2147483647</definedName>
     <definedName name="solver_num" localSheetId="0" hidden="1">4</definedName>
+    <definedName name="solver_num" localSheetId="1" hidden="1">13</definedName>
+    <definedName name="solver_num" localSheetId="4" hidden="1">3</definedName>
     <definedName name="solver_opt" localSheetId="0" hidden="1">Sheet1!$J$3</definedName>
+    <definedName name="solver_opt" localSheetId="1" hidden="1">'Sheet1 (2)'!$P$3</definedName>
+    <definedName name="solver_opt" localSheetId="4" hidden="1">Sheet2!$AO$11</definedName>
     <definedName name="solver_pre" localSheetId="0" hidden="1">0.000001</definedName>
+    <definedName name="solver_pre" localSheetId="1" hidden="1">0.000001</definedName>
+    <definedName name="solver_pre" localSheetId="4" hidden="1">0.000001</definedName>
     <definedName name="solver_rbv" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_rbv" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_rbv" localSheetId="4" hidden="1">1</definedName>
     <definedName name="solver_rel1" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_rel1" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_rel1" localSheetId="4" hidden="1">1</definedName>
+    <definedName name="solver_rel10" localSheetId="1" hidden="1">3</definedName>
+    <definedName name="solver_rel11" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_rel12" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_rel13" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_rel2" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_rel2" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_rel2" localSheetId="4" hidden="1">2</definedName>
     <definedName name="solver_rel3" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_rel3" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_rel3" localSheetId="4" hidden="1">3</definedName>
     <definedName name="solver_rel4" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_rel4" localSheetId="1" hidden="1">3</definedName>
     <definedName name="solver_rel5" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_rel5" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_rel6" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_rel7" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_rel8" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_rel9" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_rhs1" localSheetId="0" hidden="1">Sheet1!$J$18:$M$18</definedName>
+    <definedName name="solver_rhs1" localSheetId="1" hidden="1">'Sheet1 (2)'!$P$13:$S$13</definedName>
+    <definedName name="solver_rhs1" localSheetId="4" hidden="1">Sheet2!$AR$12</definedName>
+    <definedName name="solver_rhs10" localSheetId="1" hidden="1">'Sheet1 (2)'!$P$66</definedName>
+    <definedName name="solver_rhs11" localSheetId="1" hidden="1">'Sheet1 (2)'!$P$62:$S$62</definedName>
+    <definedName name="solver_rhs12" localSheetId="1" hidden="1">'Sheet1 (2)'!$U$41:$U$44</definedName>
+    <definedName name="solver_rhs13" localSheetId="1" hidden="1">'Sheet1 (2)'!$U$8:$U$11</definedName>
     <definedName name="solver_rhs2" localSheetId="0" hidden="1">Sheet1!#REF!</definedName>
+    <definedName name="solver_rhs2" localSheetId="1" hidden="1">'Sheet1 (2)'!$P$14:$S$14</definedName>
+    <definedName name="solver_rhs2" localSheetId="4" hidden="1">Sheet2!$AR$13</definedName>
     <definedName name="solver_rhs3" localSheetId="0" hidden="1">Sheet1!#REF!</definedName>
+    <definedName name="solver_rhs3" localSheetId="1" hidden="1">'Sheet1 (2)'!$P$16:$S$16</definedName>
+    <definedName name="solver_rhs3" localSheetId="4" hidden="1">Sheet2!$AR$14</definedName>
     <definedName name="solver_rhs4" localSheetId="0" hidden="1">Sheet1!$O$8:$O$11</definedName>
+    <definedName name="solver_rhs4" localSheetId="1" hidden="1">'Sheet1 (2)'!$P$33</definedName>
     <definedName name="solver_rhs5" localSheetId="0" hidden="1">Sheet1!#REF!</definedName>
+    <definedName name="solver_rhs5" localSheetId="1" hidden="1">'Sheet1 (2)'!$P$29:$S$29</definedName>
+    <definedName name="solver_rhs6" localSheetId="1" hidden="1">'Sheet1 (2)'!$Q$66</definedName>
+    <definedName name="solver_rhs7" localSheetId="1" hidden="1">'Sheet1 (2)'!$P$46:$S$46</definedName>
+    <definedName name="solver_rhs8" localSheetId="1" hidden="1">'Sheet1 (2)'!$P$47:$S$47</definedName>
+    <definedName name="solver_rhs9" localSheetId="1" hidden="1">'Sheet1 (2)'!$P$49:$S$49</definedName>
     <definedName name="solver_rlx" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_rlx" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_rlx" localSheetId="4" hidden="1">2</definedName>
     <definedName name="solver_rsd" localSheetId="0" hidden="1">0</definedName>
+    <definedName name="solver_rsd" localSheetId="1" hidden="1">0</definedName>
+    <definedName name="solver_rsd" localSheetId="4" hidden="1">0</definedName>
     <definedName name="solver_scl" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_scl" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_scl" localSheetId="4" hidden="1">1</definedName>
     <definedName name="solver_sho" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_sho" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_sho" localSheetId="4" hidden="1">2</definedName>
     <definedName name="solver_ssz" localSheetId="0" hidden="1">100</definedName>
+    <definedName name="solver_ssz" localSheetId="1" hidden="1">100</definedName>
+    <definedName name="solver_ssz" localSheetId="4" hidden="1">100</definedName>
     <definedName name="solver_tim" localSheetId="0" hidden="1">2147483647</definedName>
+    <definedName name="solver_tim" localSheetId="1" hidden="1">2147483647</definedName>
+    <definedName name="solver_tim" localSheetId="4" hidden="1">2147483647</definedName>
     <definedName name="solver_tol" localSheetId="0" hidden="1">0.01</definedName>
+    <definedName name="solver_tol" localSheetId="1" hidden="1">0.01</definedName>
+    <definedName name="solver_tol" localSheetId="4" hidden="1">0.01</definedName>
     <definedName name="solver_typ" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_typ" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_typ" localSheetId="4" hidden="1">2</definedName>
     <definedName name="solver_val" localSheetId="0" hidden="1">0</definedName>
+    <definedName name="solver_val" localSheetId="1" hidden="1">0</definedName>
+    <definedName name="solver_val" localSheetId="4" hidden="1">0</definedName>
     <definedName name="solver_ver" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_ver" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_ver" localSheetId="4" hidden="1">2</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -69,7 +172,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="72">
   <si>
     <t>Blumenau</t>
   </si>
@@ -183,6 +286,108 @@
   </si>
   <si>
     <t>x3:</t>
+  </si>
+  <si>
+    <t>&lt;=</t>
+  </si>
+  <si>
+    <t>=</t>
+  </si>
+  <si>
+    <t>&gt;=</t>
+  </si>
+  <si>
+    <t>u_f'ft</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>v_f't</t>
+  </si>
+  <si>
+    <t>y_ft</t>
+  </si>
+  <si>
+    <t>v_ft</t>
+  </si>
+  <si>
+    <t>f1</t>
+  </si>
+  <si>
+    <t>f2</t>
+  </si>
+  <si>
+    <t>f3</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>e'</t>
+  </si>
+  <si>
+    <t>total</t>
+  </si>
+  <si>
+    <t>w'_ft</t>
+  </si>
+  <si>
+    <t>e_ft</t>
+  </si>
+  <si>
+    <t>demanda</t>
+  </si>
+  <si>
+    <t>custo</t>
+  </si>
+  <si>
+    <t>CEb_f</t>
+  </si>
+  <si>
+    <t>CEp_f</t>
+  </si>
+  <si>
+    <t>sum(e_ft)</t>
+  </si>
+  <si>
+    <t>e'_ft</t>
+  </si>
+  <si>
+    <t>FO:</t>
+  </si>
+  <si>
+    <t>Ep_f</t>
+  </si>
+  <si>
+    <t>B &lt;= A*A</t>
+  </si>
+  <si>
+    <t>3 &lt;= 2*2</t>
+  </si>
+  <si>
+    <t>sum(e'_ft)</t>
+  </si>
+  <si>
+    <t>Saldo</t>
+  </si>
+  <si>
+    <t>Prod. Total</t>
+  </si>
+  <si>
+    <t>Prev. Venda</t>
+  </si>
+  <si>
+    <t>Dif</t>
+  </si>
+  <si>
+    <t>Prod. Acum</t>
+  </si>
+  <si>
+    <t>Prev. Acum</t>
+  </si>
+  <si>
+    <t>Dem. Ok</t>
   </si>
 </sst>
 </file>
@@ -206,7 +411,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -249,8 +454,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="15">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -414,11 +625,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -604,6 +828,39 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -971,8 +1228,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E815347-2441-FC41-8C00-899FDABFDCBB}">
   <dimension ref="C3:O47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+    <sheetView topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="J42" sqref="J42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2060,19 +2317,1799 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C8D0DC1-1099-834F-A649-D4073562A5D6}">
+  <dimension ref="C2:W69"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="6" max="6" width="10.83203125" style="1"/>
+    <col min="7" max="7" width="10.83203125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="13.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.5" style="1" customWidth="1"/>
+    <col min="10" max="23" width="10.83203125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="3:22" x14ac:dyDescent="0.2">
+      <c r="P2" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="3:22" x14ac:dyDescent="0.2">
+      <c r="O3" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="P3" s="73">
+        <f>V11+V14+V17+V23+V30+V44+V47+V50+V56+V63</f>
+        <v>27180000</v>
+      </c>
+    </row>
+    <row r="6" spans="3:22" x14ac:dyDescent="0.2">
+      <c r="O6" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="P6" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="3:22" x14ac:dyDescent="0.2">
+      <c r="C7" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="E7" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="F7" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="G7" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="O7" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="P7" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="R7" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="S7" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="T7" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="U7" s="16" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="3:22" x14ac:dyDescent="0.2">
+      <c r="C8" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" s="34">
+        <v>10.8</v>
+      </c>
+      <c r="E8" s="34">
+        <v>12</v>
+      </c>
+      <c r="F8" s="34">
+        <v>7.2</v>
+      </c>
+      <c r="G8" s="35">
+        <v>26</v>
+      </c>
+      <c r="O8" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="P8" s="21">
+        <v>16000</v>
+      </c>
+      <c r="Q8" s="21">
+        <v>0</v>
+      </c>
+      <c r="R8" s="21">
+        <v>194000</v>
+      </c>
+      <c r="S8" s="64">
+        <v>0</v>
+      </c>
+      <c r="T8" s="70">
+        <f>SUM(P8:S8)</f>
+        <v>210000</v>
+      </c>
+      <c r="U8" s="68">
+        <f>VLOOKUP(P6,$C$25:$G$37,2,0)</f>
+        <v>230000</v>
+      </c>
+    </row>
+    <row r="9" spans="3:22" x14ac:dyDescent="0.2">
+      <c r="C9" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" s="34">
+        <v>3.6</v>
+      </c>
+      <c r="E9" s="34">
+        <v>4</v>
+      </c>
+      <c r="F9" s="34">
+        <v>6.8</v>
+      </c>
+      <c r="G9" s="35">
+        <v>25.2</v>
+      </c>
+      <c r="O9" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="P9" s="21">
+        <v>8000</v>
+      </c>
+      <c r="Q9" s="21">
+        <v>112000</v>
+      </c>
+      <c r="R9" s="21">
+        <v>0</v>
+      </c>
+      <c r="S9" s="64">
+        <v>0</v>
+      </c>
+      <c r="T9" s="43">
+        <f t="shared" ref="T9:T11" si="0">SUM(P9:S9)</f>
+        <v>120000</v>
+      </c>
+      <c r="U9" s="68">
+        <f>VLOOKUP(P6,$C$25:$G$37,3,0)</f>
+        <v>120000</v>
+      </c>
+    </row>
+    <row r="10" spans="3:22" x14ac:dyDescent="0.2">
+      <c r="C10" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="34">
+        <v>10.8</v>
+      </c>
+      <c r="E10" s="34">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="F10" s="34">
+        <v>14.4</v>
+      </c>
+      <c r="G10" s="35">
+        <v>21.6</v>
+      </c>
+      <c r="O10" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="P10" s="21">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="21">
+        <v>74000</v>
+      </c>
+      <c r="R10" s="21">
+        <v>0</v>
+      </c>
+      <c r="S10" s="64">
+        <v>136000</v>
+      </c>
+      <c r="T10" s="43">
+        <f t="shared" si="0"/>
+        <v>210000</v>
+      </c>
+      <c r="U10" s="68">
+        <f>VLOOKUP(P6,$C$25:$G$37,4,0)</f>
+        <v>210000</v>
+      </c>
+      <c r="V10" s="16" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="11" spans="3:22" x14ac:dyDescent="0.2">
+      <c r="C11" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" s="36">
+        <v>16.399999999999999</v>
+      </c>
+      <c r="E11" s="36">
+        <v>14.8</v>
+      </c>
+      <c r="F11" s="36">
+        <v>23.4</v>
+      </c>
+      <c r="G11" s="37">
+        <v>10.8</v>
+      </c>
+      <c r="O11" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="P11" s="60">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="60">
+        <v>0</v>
+      </c>
+      <c r="R11" s="60">
+        <v>0</v>
+      </c>
+      <c r="S11" s="65">
+        <v>0</v>
+      </c>
+      <c r="T11" s="44">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="U11" s="69">
+        <f>VLOOKUP(P6,$C$25:$G$37,5,0)</f>
+        <v>0</v>
+      </c>
+      <c r="V11" s="71">
+        <f>SUMPRODUCT($D$8:$G$11,P8:S11)</f>
+        <v>5664800</v>
+      </c>
+    </row>
+    <row r="13" spans="3:22" x14ac:dyDescent="0.2">
+      <c r="C13" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="E13" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="F13" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="G13" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="O13" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="P13" s="32">
+        <v>1500000</v>
+      </c>
+      <c r="Q13" s="32">
+        <v>750000</v>
+      </c>
+      <c r="R13" s="32">
+        <v>1250000</v>
+      </c>
+      <c r="S13" s="33">
+        <v>1000000</v>
+      </c>
+      <c r="V13" s="16" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="14" spans="3:22" x14ac:dyDescent="0.2">
+      <c r="C14" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="D14" s="34">
+        <v>0</v>
+      </c>
+      <c r="E14" s="34">
+        <v>7.2</v>
+      </c>
+      <c r="F14" s="34">
+        <v>8.4</v>
+      </c>
+      <c r="G14" s="35">
+        <v>18.399999999999999</v>
+      </c>
+      <c r="O14" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="P14" s="13">
+        <f>SUM(P8:P11)</f>
+        <v>24000</v>
+      </c>
+      <c r="Q14" s="13">
+        <f t="shared" ref="Q14:S14" si="1">SUM(Q8:Q11)</f>
+        <v>186000</v>
+      </c>
+      <c r="R14" s="13">
+        <f t="shared" si="1"/>
+        <v>194000</v>
+      </c>
+      <c r="S14" s="14">
+        <f t="shared" si="1"/>
+        <v>136000</v>
+      </c>
+      <c r="V14" s="71">
+        <f>SUMPRODUCT($D$19:$G$19,P14:S14)</f>
+        <v>3742400</v>
+      </c>
+    </row>
+    <row r="15" spans="3:22" x14ac:dyDescent="0.2">
+      <c r="C15" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="D15" s="34">
+        <v>7.2</v>
+      </c>
+      <c r="E15" s="34">
+        <v>0</v>
+      </c>
+      <c r="F15" s="34">
+        <v>10</v>
+      </c>
+      <c r="G15" s="35">
+        <v>17.2</v>
+      </c>
+    </row>
+    <row r="16" spans="3:22" x14ac:dyDescent="0.2">
+      <c r="C16" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="D16" s="34">
+        <v>8.4</v>
+      </c>
+      <c r="E16" s="34">
+        <v>10</v>
+      </c>
+      <c r="F16" s="34">
+        <v>0</v>
+      </c>
+      <c r="G16" s="35">
+        <v>22.8</v>
+      </c>
+      <c r="O16" s="46" t="s">
+        <v>25</v>
+      </c>
+      <c r="P16" s="32">
+        <v>24000</v>
+      </c>
+      <c r="Q16" s="32">
+        <v>180000</v>
+      </c>
+      <c r="R16" s="32">
+        <v>160000</v>
+      </c>
+      <c r="S16" s="33">
+        <v>170000</v>
+      </c>
+      <c r="V16" s="16" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="17" spans="3:22" x14ac:dyDescent="0.2">
+      <c r="C17" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="D17" s="36">
+        <v>18.399999999999999</v>
+      </c>
+      <c r="E17" s="36">
+        <v>17.2</v>
+      </c>
+      <c r="F17" s="36">
+        <v>22.8</v>
+      </c>
+      <c r="G17" s="37">
+        <v>0</v>
+      </c>
+      <c r="O17" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="P17" s="30">
+        <v>24000</v>
+      </c>
+      <c r="Q17" s="30">
+        <v>116000</v>
+      </c>
+      <c r="R17" s="30">
+        <v>160000</v>
+      </c>
+      <c r="S17" s="67">
+        <v>0</v>
+      </c>
+      <c r="V17" s="71">
+        <f>SUMPRODUCT($D$21:$G$21,P17:S17)</f>
+        <v>3237600</v>
+      </c>
+    </row>
+    <row r="19" spans="3:22" x14ac:dyDescent="0.2">
+      <c r="C19" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="D19" s="32">
+        <v>8.1</v>
+      </c>
+      <c r="E19" s="32">
+        <v>7.2</v>
+      </c>
+      <c r="F19" s="32">
+        <v>7.6</v>
+      </c>
+      <c r="G19" s="33">
+        <v>5.4</v>
+      </c>
+      <c r="O19" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="P19" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q19" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="R19" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="S19" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="T19" s="16" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="20" spans="3:22" x14ac:dyDescent="0.2">
+      <c r="O20" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="P20" s="21">
+        <v>0</v>
+      </c>
+      <c r="Q20" s="21">
+        <v>0</v>
+      </c>
+      <c r="R20" s="21">
+        <v>0</v>
+      </c>
+      <c r="S20" s="64">
+        <v>0</v>
+      </c>
+      <c r="T20" s="43">
+        <f>SUM(P20:S20)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="3:22" x14ac:dyDescent="0.2">
+      <c r="C21" s="46" t="s">
+        <v>23</v>
+      </c>
+      <c r="D21" s="32">
+        <v>10.3</v>
+      </c>
+      <c r="E21" s="32">
+        <v>12.4</v>
+      </c>
+      <c r="F21" s="32">
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="G21" s="33">
+        <v>10.5</v>
+      </c>
+      <c r="O21" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="P21" s="21">
+        <v>0</v>
+      </c>
+      <c r="Q21" s="21">
+        <v>0</v>
+      </c>
+      <c r="R21" s="21">
+        <v>0</v>
+      </c>
+      <c r="S21" s="64">
+        <v>0</v>
+      </c>
+      <c r="T21" s="43">
+        <f t="shared" ref="T21:T23" si="2">SUM(P21:S21)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="3:22" x14ac:dyDescent="0.2">
+      <c r="O22" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="P22" s="21">
+        <v>0</v>
+      </c>
+      <c r="Q22" s="21">
+        <v>0</v>
+      </c>
+      <c r="R22" s="21">
+        <v>0</v>
+      </c>
+      <c r="S22" s="64">
+        <v>0</v>
+      </c>
+      <c r="T22" s="43">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="V22" s="16" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="23" spans="3:22" x14ac:dyDescent="0.2">
+      <c r="C23" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="D23" s="32">
+        <v>5.3</v>
+      </c>
+      <c r="E23" s="32">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="F23" s="32">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="G23" s="33">
+        <v>3.8</v>
+      </c>
+      <c r="O23" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="P23" s="60">
+        <v>0</v>
+      </c>
+      <c r="Q23" s="60">
+        <v>0</v>
+      </c>
+      <c r="R23" s="60">
+        <v>0</v>
+      </c>
+      <c r="S23" s="65">
+        <v>0</v>
+      </c>
+      <c r="T23" s="44">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="V23" s="71">
+        <f>SUMPRODUCT($D$14:$G$17,P20:S23)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="3:22" x14ac:dyDescent="0.2">
+      <c r="C25" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="D25" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="E25" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="F25" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="G25" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="H25" s="66" t="s">
+        <v>66</v>
+      </c>
+      <c r="I25" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="J25" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="K25" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="L25" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="M25" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="O25" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="P25" s="13">
+        <f>T20</f>
+        <v>0</v>
+      </c>
+      <c r="Q25" s="13">
+        <f>T21</f>
+        <v>0</v>
+      </c>
+      <c r="R25" s="13">
+        <f>T22</f>
+        <v>0</v>
+      </c>
+      <c r="S25" s="14">
+        <f>T23</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="3:22" x14ac:dyDescent="0.2">
+      <c r="C26" s="19">
+        <v>1</v>
+      </c>
+      <c r="D26" s="38">
+        <v>230000</v>
+      </c>
+      <c r="E26" s="39">
+        <v>120000</v>
+      </c>
+      <c r="F26" s="39">
+        <v>210000</v>
+      </c>
+      <c r="G26" s="40">
+        <v>0</v>
+      </c>
+      <c r="H26" s="1">
+        <f>SUM(D26:G26)</f>
+        <v>560000</v>
+      </c>
+      <c r="I26" s="1">
+        <v>300000</v>
+      </c>
+      <c r="J26" s="1">
+        <f>H26</f>
+        <v>560000</v>
+      </c>
+      <c r="K26" s="1">
+        <f>I26</f>
+        <v>300000</v>
+      </c>
+      <c r="L26" s="1">
+        <f>J26-K26</f>
+        <v>260000</v>
+      </c>
+      <c r="M26" s="1">
+        <f>I26</f>
+        <v>300000</v>
+      </c>
+    </row>
+    <row r="27" spans="3:22" x14ac:dyDescent="0.2">
+      <c r="C27" s="19">
+        <v>2</v>
+      </c>
+      <c r="D27" s="41">
+        <v>150000</v>
+      </c>
+      <c r="E27" s="34">
+        <v>0</v>
+      </c>
+      <c r="F27" s="34">
+        <v>110000</v>
+      </c>
+      <c r="G27" s="35">
+        <v>0</v>
+      </c>
+      <c r="H27" s="1">
+        <f t="shared" ref="H27:H37" si="3">SUM(D27:G27)</f>
+        <v>260000</v>
+      </c>
+      <c r="I27" s="1">
+        <v>500000</v>
+      </c>
+      <c r="J27" s="1">
+        <f>H27+J26</f>
+        <v>820000</v>
+      </c>
+      <c r="K27" s="1">
+        <f>I27+K26</f>
+        <v>800000</v>
+      </c>
+      <c r="L27" s="1">
+        <f>J27-K27</f>
+        <v>20000</v>
+      </c>
+      <c r="M27" s="1">
+        <f>I27</f>
+        <v>500000</v>
+      </c>
+      <c r="O27" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="P27" s="13">
+        <f>P14-P17-P25</f>
+        <v>0</v>
+      </c>
+      <c r="Q27" s="13">
+        <f>Q14-Q17-Q25</f>
+        <v>70000</v>
+      </c>
+      <c r="R27" s="13">
+        <f>R14-R17-R25</f>
+        <v>34000</v>
+      </c>
+      <c r="S27" s="14">
+        <f>S14-S17-S25</f>
+        <v>136000</v>
+      </c>
+    </row>
+    <row r="28" spans="3:22" x14ac:dyDescent="0.2">
+      <c r="C28" s="19">
+        <v>3</v>
+      </c>
+      <c r="D28" s="41">
+        <v>0</v>
+      </c>
+      <c r="E28" s="34">
+        <v>0</v>
+      </c>
+      <c r="F28" s="34">
+        <v>0</v>
+      </c>
+      <c r="G28" s="35">
+        <v>0</v>
+      </c>
+      <c r="H28" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="I28" s="1">
+        <v>700000</v>
+      </c>
+      <c r="J28" s="1">
+        <f t="shared" ref="J28:J37" si="4">H28+J27</f>
+        <v>820000</v>
+      </c>
+      <c r="K28" s="1">
+        <f t="shared" ref="K28:K37" si="5">I28+K27</f>
+        <v>1500000</v>
+      </c>
+      <c r="L28" s="1">
+        <f>J28-K28</f>
+        <v>-680000</v>
+      </c>
+      <c r="M28" s="1">
+        <f>I28+L28</f>
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="29" spans="3:22" x14ac:dyDescent="0.2">
+      <c r="C29" s="19">
+        <v>4</v>
+      </c>
+      <c r="D29" s="41">
+        <v>0</v>
+      </c>
+      <c r="E29" s="34">
+        <v>0</v>
+      </c>
+      <c r="F29" s="34">
+        <v>0</v>
+      </c>
+      <c r="G29" s="35">
+        <v>0</v>
+      </c>
+      <c r="H29" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="I29" s="1">
+        <v>900000</v>
+      </c>
+      <c r="J29" s="1">
+        <f t="shared" si="4"/>
+        <v>820000</v>
+      </c>
+      <c r="K29" s="1">
+        <f t="shared" si="5"/>
+        <v>2400000</v>
+      </c>
+      <c r="O29" s="46" t="s">
+        <v>61</v>
+      </c>
+      <c r="P29" s="32">
+        <v>1000000</v>
+      </c>
+      <c r="Q29" s="32">
+        <v>800000</v>
+      </c>
+      <c r="R29" s="32">
+        <v>1000000</v>
+      </c>
+      <c r="S29" s="33">
+        <v>900000</v>
+      </c>
+      <c r="V29" s="16" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="30" spans="3:22" x14ac:dyDescent="0.2">
+      <c r="C30" s="19">
+        <v>5</v>
+      </c>
+      <c r="D30" s="41">
+        <v>0</v>
+      </c>
+      <c r="E30" s="34">
+        <v>0</v>
+      </c>
+      <c r="F30" s="34">
+        <v>0</v>
+      </c>
+      <c r="G30" s="35">
+        <v>100000</v>
+      </c>
+      <c r="H30" s="1">
+        <f t="shared" si="3"/>
+        <v>100000</v>
+      </c>
+      <c r="I30" s="1">
+        <v>800000</v>
+      </c>
+      <c r="J30" s="1">
+        <f t="shared" si="4"/>
+        <v>920000</v>
+      </c>
+      <c r="K30" s="1">
+        <f t="shared" si="5"/>
+        <v>3200000</v>
+      </c>
+      <c r="O30" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="P30" s="13">
+        <f>P17</f>
+        <v>24000</v>
+      </c>
+      <c r="Q30" s="13">
+        <f>Q17</f>
+        <v>116000</v>
+      </c>
+      <c r="R30" s="13">
+        <f>R17</f>
+        <v>160000</v>
+      </c>
+      <c r="S30" s="14">
+        <f>S17</f>
+        <v>0</v>
+      </c>
+      <c r="V30" s="71">
+        <f>SUMPRODUCT($D$23:$G$23,P30:S30)</f>
+        <v>1338800</v>
+      </c>
+    </row>
+    <row r="31" spans="3:22" x14ac:dyDescent="0.2">
+      <c r="C31" s="19">
+        <v>6</v>
+      </c>
+      <c r="D31" s="41">
+        <v>0</v>
+      </c>
+      <c r="E31" s="34">
+        <v>110000</v>
+      </c>
+      <c r="F31" s="34">
+        <v>0</v>
+      </c>
+      <c r="G31" s="35">
+        <v>110000</v>
+      </c>
+      <c r="H31" s="1">
+        <f t="shared" si="3"/>
+        <v>220000</v>
+      </c>
+      <c r="I31" s="1">
+        <v>800000</v>
+      </c>
+      <c r="J31" s="1">
+        <f t="shared" si="4"/>
+        <v>1140000</v>
+      </c>
+      <c r="K31" s="1">
+        <f t="shared" si="5"/>
+        <v>4000000</v>
+      </c>
+    </row>
+    <row r="32" spans="3:22" x14ac:dyDescent="0.2">
+      <c r="C32" s="19">
+        <v>7</v>
+      </c>
+      <c r="D32" s="41">
+        <v>140000</v>
+      </c>
+      <c r="E32" s="34">
+        <v>250000</v>
+      </c>
+      <c r="F32" s="34">
+        <v>130000</v>
+      </c>
+      <c r="G32" s="35">
+        <v>150000</v>
+      </c>
+      <c r="H32" s="1">
+        <f t="shared" si="3"/>
+        <v>670000</v>
+      </c>
+      <c r="I32" s="1">
+        <v>700000</v>
+      </c>
+      <c r="J32" s="1">
+        <f t="shared" si="4"/>
+        <v>1810000</v>
+      </c>
+      <c r="K32" s="1">
+        <f t="shared" si="5"/>
+        <v>4700000</v>
+      </c>
+      <c r="O32" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="P32" s="71">
+        <f>SUM(P30:S30)</f>
+        <v>300000</v>
+      </c>
+      <c r="Q32" s="16" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="33" spans="3:22" x14ac:dyDescent="0.2">
+      <c r="C33" s="19">
+        <v>8</v>
+      </c>
+      <c r="D33" s="41">
+        <v>180000</v>
+      </c>
+      <c r="E33" s="34">
+        <v>360000</v>
+      </c>
+      <c r="F33" s="34">
+        <v>240000</v>
+      </c>
+      <c r="G33" s="35">
+        <v>250000</v>
+      </c>
+      <c r="H33" s="1">
+        <f t="shared" si="3"/>
+        <v>1030000</v>
+      </c>
+      <c r="I33" s="1">
+        <v>600000</v>
+      </c>
+      <c r="J33" s="1">
+        <f t="shared" si="4"/>
+        <v>2840000</v>
+      </c>
+      <c r="K33" s="1">
+        <f t="shared" si="5"/>
+        <v>5300000</v>
+      </c>
+      <c r="O33" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="P33" s="72">
+        <v>300000</v>
+      </c>
+      <c r="Q33" s="71">
+        <f>P32-P33</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="3:22" x14ac:dyDescent="0.2">
+      <c r="C34" s="19">
+        <v>9</v>
+      </c>
+      <c r="D34" s="41">
+        <v>260000</v>
+      </c>
+      <c r="E34" s="34">
+        <v>380000</v>
+      </c>
+      <c r="F34" s="34">
+        <v>370000</v>
+      </c>
+      <c r="G34" s="35">
+        <v>260000</v>
+      </c>
+      <c r="H34" s="1">
+        <f t="shared" si="3"/>
+        <v>1270000</v>
+      </c>
+      <c r="I34" s="1">
+        <v>600000</v>
+      </c>
+      <c r="J34" s="1">
+        <f t="shared" si="4"/>
+        <v>4110000</v>
+      </c>
+      <c r="K34" s="1">
+        <f t="shared" si="5"/>
+        <v>5900000</v>
+      </c>
+    </row>
+    <row r="35" spans="3:22" x14ac:dyDescent="0.2">
+      <c r="C35" s="19">
+        <v>10</v>
+      </c>
+      <c r="D35" s="41">
+        <v>280000</v>
+      </c>
+      <c r="E35" s="34">
+        <v>370000</v>
+      </c>
+      <c r="F35" s="34">
+        <v>400000</v>
+      </c>
+      <c r="G35" s="35">
+        <v>250000</v>
+      </c>
+      <c r="H35" s="1">
+        <f t="shared" si="3"/>
+        <v>1300000</v>
+      </c>
+      <c r="I35" s="1">
+        <v>500000</v>
+      </c>
+      <c r="J35" s="1">
+        <f t="shared" si="4"/>
+        <v>5410000</v>
+      </c>
+      <c r="K35" s="1">
+        <f t="shared" si="5"/>
+        <v>6400000</v>
+      </c>
+      <c r="O35" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="P35" s="30">
+        <v>0</v>
+      </c>
+      <c r="Q35" s="30">
+        <v>0</v>
+      </c>
+      <c r="R35" s="30">
+        <v>0</v>
+      </c>
+      <c r="S35" s="67">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="3:22" x14ac:dyDescent="0.2">
+      <c r="C36" s="19">
+        <v>11</v>
+      </c>
+      <c r="D36" s="41">
+        <v>380000</v>
+      </c>
+      <c r="E36" s="34">
+        <v>350000</v>
+      </c>
+      <c r="F36" s="34">
+        <v>420000</v>
+      </c>
+      <c r="G36" s="35">
+        <v>200000</v>
+      </c>
+      <c r="H36" s="1">
+        <f t="shared" si="3"/>
+        <v>1350000</v>
+      </c>
+      <c r="I36" s="1">
+        <v>500000</v>
+      </c>
+      <c r="J36" s="1">
+        <f t="shared" si="4"/>
+        <v>6760000</v>
+      </c>
+      <c r="K36" s="1">
+        <f t="shared" si="5"/>
+        <v>6900000</v>
+      </c>
+      <c r="O36" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="P36" s="71">
+        <f>SUM(P35:S35)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="3:22" x14ac:dyDescent="0.2">
+      <c r="C37" s="20">
+        <v>12</v>
+      </c>
+      <c r="D37" s="42">
+        <v>350000</v>
+      </c>
+      <c r="E37" s="36">
+        <v>230000</v>
+      </c>
+      <c r="F37" s="36">
+        <v>380000</v>
+      </c>
+      <c r="G37" s="37">
+        <v>120000</v>
+      </c>
+      <c r="H37" s="1">
+        <f t="shared" si="3"/>
+        <v>1080000</v>
+      </c>
+      <c r="I37" s="1">
+        <v>400000</v>
+      </c>
+      <c r="J37" s="1">
+        <f t="shared" si="4"/>
+        <v>7840000</v>
+      </c>
+      <c r="K37" s="1">
+        <f t="shared" si="5"/>
+        <v>7300000</v>
+      </c>
+    </row>
+    <row r="38" spans="3:22" x14ac:dyDescent="0.2">
+      <c r="F38"/>
+      <c r="G38"/>
+    </row>
+    <row r="39" spans="3:22" x14ac:dyDescent="0.2">
+      <c r="F39"/>
+      <c r="G39"/>
+      <c r="O39" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="P39" s="12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="3:22" x14ac:dyDescent="0.2">
+      <c r="F40"/>
+      <c r="G40"/>
+      <c r="O40" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="P40" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q40" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="R40" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="S40" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="T40" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="U40" s="16" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="41" spans="3:22" x14ac:dyDescent="0.2">
+      <c r="F41"/>
+      <c r="G41"/>
+      <c r="O41" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="P41" s="21">
+        <v>24000</v>
+      </c>
+      <c r="Q41" s="21">
+        <v>0</v>
+      </c>
+      <c r="R41" s="21">
+        <v>126000</v>
+      </c>
+      <c r="S41" s="64">
+        <v>0</v>
+      </c>
+      <c r="T41" s="70">
+        <f>SUM(P41:S41)</f>
+        <v>150000</v>
+      </c>
+      <c r="U41" s="68">
+        <f>VLOOKUP(P39,$C$25:$G$37,2,0)</f>
+        <v>150000</v>
+      </c>
+    </row>
+    <row r="42" spans="3:22" x14ac:dyDescent="0.2">
+      <c r="F42"/>
+      <c r="G42"/>
+      <c r="O42" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="P42" s="21">
+        <v>0</v>
+      </c>
+      <c r="Q42" s="21">
+        <v>0</v>
+      </c>
+      <c r="R42" s="21">
+        <v>0</v>
+      </c>
+      <c r="S42" s="64">
+        <v>0</v>
+      </c>
+      <c r="T42" s="43">
+        <f t="shared" ref="T42:T44" si="6">SUM(P42:S42)</f>
+        <v>0</v>
+      </c>
+      <c r="U42" s="68">
+        <f>VLOOKUP(P39,$C$25:$G$37,3,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="3:22" x14ac:dyDescent="0.2">
+      <c r="F43"/>
+      <c r="G43"/>
+      <c r="O43" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="P43" s="21">
+        <v>0</v>
+      </c>
+      <c r="Q43" s="21">
+        <v>110000</v>
+      </c>
+      <c r="R43" s="21">
+        <v>0</v>
+      </c>
+      <c r="S43" s="64">
+        <v>0</v>
+      </c>
+      <c r="T43" s="43">
+        <f t="shared" si="6"/>
+        <v>110000</v>
+      </c>
+      <c r="U43" s="68">
+        <f>VLOOKUP(P39,$C$25:$G$37,4,0)</f>
+        <v>110000</v>
+      </c>
+      <c r="V43" s="16" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="44" spans="3:22" x14ac:dyDescent="0.2">
+      <c r="F44"/>
+      <c r="G44"/>
+      <c r="O44" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="P44" s="60">
+        <v>0</v>
+      </c>
+      <c r="Q44" s="60">
+        <v>0</v>
+      </c>
+      <c r="R44" s="60">
+        <v>0</v>
+      </c>
+      <c r="S44" s="65">
+        <v>0</v>
+      </c>
+      <c r="T44" s="44">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="U44" s="69">
+        <f>VLOOKUP(P39,$C$25:$G$37,5,0)</f>
+        <v>0</v>
+      </c>
+      <c r="V44" s="71">
+        <f>SUMPRODUCT($D$8:$G$11,P41:S44)</f>
+        <v>2178400</v>
+      </c>
+    </row>
+    <row r="45" spans="3:22" x14ac:dyDescent="0.2">
+      <c r="F45"/>
+      <c r="G45"/>
+    </row>
+    <row r="46" spans="3:22" x14ac:dyDescent="0.2">
+      <c r="F46"/>
+      <c r="G46"/>
+      <c r="O46" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="P46" s="32">
+        <v>1500000</v>
+      </c>
+      <c r="Q46" s="32">
+        <v>750000</v>
+      </c>
+      <c r="R46" s="32">
+        <v>1250000</v>
+      </c>
+      <c r="S46" s="33">
+        <v>1000000</v>
+      </c>
+      <c r="V46" s="16" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="47" spans="3:22" x14ac:dyDescent="0.2">
+      <c r="O47" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="P47" s="13">
+        <f>P27+SUM(P20:P23)+SUM(P41:P44)</f>
+        <v>24000</v>
+      </c>
+      <c r="Q47" s="13">
+        <f t="shared" ref="Q47:S47" si="7">Q27+SUM(Q20:Q23)+SUM(Q41:Q44)</f>
+        <v>180000</v>
+      </c>
+      <c r="R47" s="13">
+        <f>R27+SUM(R20:R23)+SUM(R41:R44)</f>
+        <v>160000</v>
+      </c>
+      <c r="S47" s="14">
+        <f t="shared" si="7"/>
+        <v>136000</v>
+      </c>
+      <c r="V47" s="71">
+        <f>SUMPRODUCT($D$19:$G$19,P47:S47)</f>
+        <v>3440800</v>
+      </c>
+    </row>
+    <row r="49" spans="15:22" x14ac:dyDescent="0.2">
+      <c r="O49" s="46" t="s">
+        <v>25</v>
+      </c>
+      <c r="P49" s="32">
+        <v>24000</v>
+      </c>
+      <c r="Q49" s="32">
+        <v>180000</v>
+      </c>
+      <c r="R49" s="32">
+        <v>160000</v>
+      </c>
+      <c r="S49" s="33">
+        <v>170000</v>
+      </c>
+      <c r="V49" s="16" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="50" spans="15:22" x14ac:dyDescent="0.2">
+      <c r="O50" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="P50" s="30">
+        <v>24000</v>
+      </c>
+      <c r="Q50" s="30">
+        <v>180000</v>
+      </c>
+      <c r="R50" s="30">
+        <v>160000</v>
+      </c>
+      <c r="S50" s="67">
+        <v>136000</v>
+      </c>
+      <c r="V50" s="71">
+        <f>SUMPRODUCT($D$21:$G$21,P50:S50)</f>
+        <v>5459200</v>
+      </c>
+    </row>
+    <row r="52" spans="15:22" x14ac:dyDescent="0.2">
+      <c r="O52" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="P52" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q52" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="R52" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="S52" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="T52" s="16" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="53" spans="15:22" x14ac:dyDescent="0.2">
+      <c r="O53" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="P53" s="21">
+        <v>0</v>
+      </c>
+      <c r="Q53" s="21">
+        <v>0</v>
+      </c>
+      <c r="R53" s="21">
+        <v>0</v>
+      </c>
+      <c r="S53" s="64">
+        <v>0</v>
+      </c>
+      <c r="T53" s="43">
+        <f>SUM(P53:S53)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="15:22" x14ac:dyDescent="0.2">
+      <c r="O54" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="P54" s="21">
+        <v>0</v>
+      </c>
+      <c r="Q54" s="21">
+        <v>0</v>
+      </c>
+      <c r="R54" s="21">
+        <v>0</v>
+      </c>
+      <c r="S54" s="64">
+        <v>0</v>
+      </c>
+      <c r="T54" s="43">
+        <f t="shared" ref="T54:T56" si="8">SUM(P54:S54)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="15:22" x14ac:dyDescent="0.2">
+      <c r="O55" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="P55" s="21">
+        <v>0</v>
+      </c>
+      <c r="Q55" s="21">
+        <v>0</v>
+      </c>
+      <c r="R55" s="21">
+        <v>0</v>
+      </c>
+      <c r="S55" s="64">
+        <v>0</v>
+      </c>
+      <c r="T55" s="43">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="V55" s="16" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="56" spans="15:22" x14ac:dyDescent="0.2">
+      <c r="O56" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="P56" s="60">
+        <v>0</v>
+      </c>
+      <c r="Q56" s="60">
+        <v>0</v>
+      </c>
+      <c r="R56" s="60">
+        <v>0</v>
+      </c>
+      <c r="S56" s="65">
+        <v>0</v>
+      </c>
+      <c r="T56" s="44">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="V56" s="71">
+        <f>SUMPRODUCT($D$14:$G$17,P53:S56)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="15:22" x14ac:dyDescent="0.2">
+      <c r="O58" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="P58" s="13">
+        <f>T53</f>
+        <v>0</v>
+      </c>
+      <c r="Q58" s="13">
+        <f>T54</f>
+        <v>0</v>
+      </c>
+      <c r="R58" s="13">
+        <f>T55</f>
+        <v>0</v>
+      </c>
+      <c r="S58" s="14">
+        <f>T56</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="15:22" x14ac:dyDescent="0.2">
+      <c r="O60" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="P60" s="13">
+        <f>P47-P50-P58</f>
+        <v>0</v>
+      </c>
+      <c r="Q60" s="13">
+        <f>Q47-Q50-Q58</f>
+        <v>0</v>
+      </c>
+      <c r="R60" s="13">
+        <f>R47-R50-R58</f>
+        <v>0</v>
+      </c>
+      <c r="S60" s="14">
+        <f>S47-S50-S58</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="15:22" x14ac:dyDescent="0.2">
+      <c r="O62" s="46" t="s">
+        <v>61</v>
+      </c>
+      <c r="P62" s="32">
+        <v>1000000</v>
+      </c>
+      <c r="Q62" s="32">
+        <v>800000</v>
+      </c>
+      <c r="R62" s="32">
+        <v>1000000</v>
+      </c>
+      <c r="S62" s="33">
+        <v>900000</v>
+      </c>
+      <c r="V62" s="16" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="63" spans="15:22" x14ac:dyDescent="0.2">
+      <c r="O63" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="P63" s="13">
+        <f>P35+P50</f>
+        <v>24000</v>
+      </c>
+      <c r="Q63" s="13">
+        <f t="shared" ref="Q63:S63" si="9">Q35+Q50</f>
+        <v>180000</v>
+      </c>
+      <c r="R63" s="13">
+        <f t="shared" si="9"/>
+        <v>160000</v>
+      </c>
+      <c r="S63" s="14">
+        <f t="shared" si="9"/>
+        <v>136000</v>
+      </c>
+      <c r="V63" s="71">
+        <f>SUMPRODUCT($D$23:$G$23,P63:S63)</f>
+        <v>2118000</v>
+      </c>
+    </row>
+    <row r="65" spans="15:19" x14ac:dyDescent="0.2">
+      <c r="O65" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="P65" s="71">
+        <f>SUM(P63:S63)</f>
+        <v>500000</v>
+      </c>
+      <c r="Q65" s="16" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="66" spans="15:19" x14ac:dyDescent="0.2">
+      <c r="O66" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="P66" s="72">
+        <v>500000</v>
+      </c>
+      <c r="Q66" s="71">
+        <f>P65-P66</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="15:19" x14ac:dyDescent="0.2">
+      <c r="O68" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="P68" s="30">
+        <v>0</v>
+      </c>
+      <c r="Q68" s="30">
+        <v>0</v>
+      </c>
+      <c r="R68" s="30">
+        <v>0</v>
+      </c>
+      <c r="S68" s="67">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="15:19" x14ac:dyDescent="0.2">
+      <c r="O69" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="P69" s="71">
+        <f>SUM(P68:S68)</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB622E8B-699F-B34E-9BE3-02647CF258ED}">
+  <dimension ref="H17:H20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="17" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H17" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="20" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H20" t="s">
+        <v>63</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96BA8C6C-5B11-1E40-904E-DE6936468200}">
+  <dimension ref="G20:L27"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L20" sqref="L20:L23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="20" spans="7:12" x14ac:dyDescent="0.2">
+      <c r="G20" t="s">
+        <v>46</v>
+      </c>
+      <c r="H20">
+        <v>12</v>
+      </c>
+      <c r="I20">
+        <f>H27</f>
+        <v>38</v>
+      </c>
+      <c r="J20">
+        <f>SUM(H20:H23)</f>
+        <v>103</v>
+      </c>
+      <c r="K20">
+        <f>H20/J20</f>
+        <v>0.11650485436893204</v>
+      </c>
+      <c r="L20">
+        <f>K20*I20</f>
+        <v>4.4271844660194173</v>
+      </c>
+    </row>
+    <row r="21" spans="7:12" x14ac:dyDescent="0.2">
+      <c r="G21" t="s">
+        <v>47</v>
+      </c>
+      <c r="H21">
+        <v>45</v>
+      </c>
+      <c r="I21">
+        <f>H27</f>
+        <v>38</v>
+      </c>
+      <c r="J21">
+        <f>J20</f>
+        <v>103</v>
+      </c>
+      <c r="K21">
+        <f>H21/J21</f>
+        <v>0.43689320388349512</v>
+      </c>
+      <c r="L21">
+        <f>K21*I21</f>
+        <v>16.601941747572816</v>
+      </c>
+    </row>
+    <row r="22" spans="7:12" x14ac:dyDescent="0.2">
+      <c r="G22" t="s">
+        <v>48</v>
+      </c>
+      <c r="H22">
+        <v>17</v>
+      </c>
+      <c r="I22">
+        <f>H27</f>
+        <v>38</v>
+      </c>
+      <c r="J22">
+        <f>J21</f>
+        <v>103</v>
+      </c>
+      <c r="K22">
+        <f>H22/J22</f>
+        <v>0.1650485436893204</v>
+      </c>
+      <c r="L22">
+        <f>K22*I22</f>
+        <v>6.2718446601941755</v>
+      </c>
+    </row>
+    <row r="23" spans="7:12" x14ac:dyDescent="0.2">
+      <c r="G23" t="s">
+        <v>48</v>
+      </c>
+      <c r="H23">
+        <v>29</v>
+      </c>
+      <c r="I23">
+        <f>H27</f>
+        <v>38</v>
+      </c>
+      <c r="J23">
+        <f>J22</f>
+        <v>103</v>
+      </c>
+      <c r="K23">
+        <f>H23/J23</f>
+        <v>0.28155339805825241</v>
+      </c>
+      <c r="L23">
+        <f>K23*I23</f>
+        <v>10.699029126213592</v>
+      </c>
+    </row>
+    <row r="26" spans="7:12" x14ac:dyDescent="0.2">
+      <c r="G26" t="s">
+        <v>49</v>
+      </c>
+      <c r="H26">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="27" spans="7:12" x14ac:dyDescent="0.2">
+      <c r="G27" t="s">
+        <v>50</v>
+      </c>
+      <c r="H27">
+        <f>SUM(H20:H23)-H26</f>
+        <v>38</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0340B6A-7156-4643-BFCC-B4B1541D176F}">
-  <dimension ref="E9:M47"/>
+  <dimension ref="E9:AR47"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="91" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView topLeftCell="I1" zoomScale="91" workbookViewId="0">
+      <selection activeCell="AH61" sqref="AH61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="5" max="13" width="10.83203125" style="1"/>
+    <col min="35" max="44" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="9" spans="7:13" x14ac:dyDescent="0.2">
+    <row r="9" spans="7:44" x14ac:dyDescent="0.2">
       <c r="G9" s="51" t="s">
         <v>26</v>
       </c>
@@ -2091,8 +4128,38 @@
       <c r="L9" s="45" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="10" spans="7:13" x14ac:dyDescent="0.2">
+      <c r="Z9" s="51" t="s">
+        <v>26</v>
+      </c>
+      <c r="AA9" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="AB9" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="AC9" s="45" t="s">
+        <v>31</v>
+      </c>
+      <c r="AJ9" s="51" t="s">
+        <v>26</v>
+      </c>
+      <c r="AK9" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="AL9" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="AM9" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="AN9" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="AO9" s="45" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="7:44" x14ac:dyDescent="0.2">
       <c r="G10" s="47">
         <v>6</v>
       </c>
@@ -2111,8 +4178,34 @@
       <c r="L10" s="48">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="7:13" x14ac:dyDescent="0.2">
+      <c r="Z10" s="51">
+        <v>0</v>
+      </c>
+      <c r="AA10" s="7">
+        <v>8.5</v>
+      </c>
+      <c r="AB10" s="7">
+        <v>4.5</v>
+      </c>
+      <c r="AC10" s="45"/>
+      <c r="AJ10" s="51">
+        <v>0</v>
+      </c>
+      <c r="AK10" s="7">
+        <v>8.5</v>
+      </c>
+      <c r="AL10" s="7">
+        <v>4.5</v>
+      </c>
+      <c r="AM10" s="7">
+        <v>0</v>
+      </c>
+      <c r="AN10" s="7">
+        <v>0</v>
+      </c>
+      <c r="AO10" s="45"/>
+    </row>
+    <row r="11" spans="7:44" x14ac:dyDescent="0.2">
       <c r="G11" s="24">
         <v>2</v>
       </c>
@@ -2131,8 +4224,40 @@
       <c r="L11" s="49">
         <v>20</v>
       </c>
-    </row>
-    <row r="12" spans="7:13" x14ac:dyDescent="0.2">
+      <c r="Z11" s="47">
+        <v>6</v>
+      </c>
+      <c r="AA11" s="9">
+        <v>4</v>
+      </c>
+      <c r="AB11" s="9">
+        <v>5</v>
+      </c>
+      <c r="AC11" s="48">
+        <f>SUMPRODUCT($Z$10:$AB$10,Z11:AB11)</f>
+        <v>56.5</v>
+      </c>
+      <c r="AJ11" s="47">
+        <v>6</v>
+      </c>
+      <c r="AK11" s="9">
+        <v>4</v>
+      </c>
+      <c r="AL11" s="9">
+        <v>5</v>
+      </c>
+      <c r="AM11" s="9">
+        <v>0</v>
+      </c>
+      <c r="AN11" s="9">
+        <v>0</v>
+      </c>
+      <c r="AO11" s="48">
+        <f>SUMPRODUCT($AJ$10:$AN$10,AJ11:AN11)</f>
+        <v>56.5</v>
+      </c>
+    </row>
+    <row r="12" spans="7:44" x14ac:dyDescent="0.2">
       <c r="G12" s="24">
         <v>2</v>
       </c>
@@ -2151,8 +4276,52 @@
       <c r="L12" s="49">
         <v>60</v>
       </c>
-    </row>
-    <row r="13" spans="7:13" x14ac:dyDescent="0.2">
+      <c r="Z12" s="24">
+        <v>2</v>
+      </c>
+      <c r="AA12" s="3">
+        <v>-1</v>
+      </c>
+      <c r="AB12" s="3">
+        <v>4</v>
+      </c>
+      <c r="AC12" s="49">
+        <f t="shared" ref="AC12:AC14" si="0">SUMPRODUCT($Z$10:$AB$10,Z12:AB12)</f>
+        <v>9.5</v>
+      </c>
+      <c r="AE12" t="s">
+        <v>38</v>
+      </c>
+      <c r="AF12" s="63">
+        <v>20</v>
+      </c>
+      <c r="AJ12" s="24">
+        <v>2</v>
+      </c>
+      <c r="AK12" s="3">
+        <v>-1</v>
+      </c>
+      <c r="AL12" s="3">
+        <v>4</v>
+      </c>
+      <c r="AM12" s="3">
+        <v>1</v>
+      </c>
+      <c r="AN12" s="3">
+        <v>0</v>
+      </c>
+      <c r="AO12" s="49">
+        <f t="shared" ref="AO12:AO14" si="1">SUMPRODUCT($AJ$10:$AN$10,AJ12:AN12)</f>
+        <v>9.5</v>
+      </c>
+      <c r="AQ12" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AR12" s="63">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="7:44" x14ac:dyDescent="0.2">
       <c r="G13" s="25">
         <v>1</v>
       </c>
@@ -2174,8 +4343,98 @@
       <c r="M13" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="16" spans="7:13" x14ac:dyDescent="0.2">
+      <c r="Z13" s="24">
+        <v>2</v>
+      </c>
+      <c r="AA13" s="3">
+        <v>6</v>
+      </c>
+      <c r="AB13" s="3">
+        <v>2</v>
+      </c>
+      <c r="AC13" s="49">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+      <c r="AE13" t="s">
+        <v>39</v>
+      </c>
+      <c r="AF13" s="49">
+        <v>60</v>
+      </c>
+      <c r="AJ13" s="24">
+        <v>2</v>
+      </c>
+      <c r="AK13" s="3">
+        <v>6</v>
+      </c>
+      <c r="AL13" s="3">
+        <v>2</v>
+      </c>
+      <c r="AM13" s="3">
+        <v>0</v>
+      </c>
+      <c r="AN13" s="3">
+        <v>0</v>
+      </c>
+      <c r="AO13" s="49">
+        <f t="shared" si="1"/>
+        <v>60</v>
+      </c>
+      <c r="AQ13" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AR13" s="49">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="14" spans="7:44" x14ac:dyDescent="0.2">
+      <c r="Z14" s="25">
+        <v>1</v>
+      </c>
+      <c r="AA14" s="5">
+        <v>1</v>
+      </c>
+      <c r="AB14" s="5">
+        <v>3</v>
+      </c>
+      <c r="AC14" s="50">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="AE14" t="s">
+        <v>40</v>
+      </c>
+      <c r="AF14" s="50">
+        <v>22</v>
+      </c>
+      <c r="AJ14" s="25">
+        <v>1</v>
+      </c>
+      <c r="AK14" s="5">
+        <v>1</v>
+      </c>
+      <c r="AL14" s="5">
+        <v>3</v>
+      </c>
+      <c r="AM14" s="5">
+        <v>0</v>
+      </c>
+      <c r="AN14" s="5">
+        <v>-1</v>
+      </c>
+      <c r="AO14" s="50">
+        <f t="shared" si="1"/>
+        <v>22</v>
+      </c>
+      <c r="AQ14" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AR14" s="50">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="7:44" x14ac:dyDescent="0.2">
       <c r="G16" s="51" t="s">
         <v>26</v>
       </c>
@@ -2261,23 +4520,23 @@
         <v>-1</v>
       </c>
       <c r="H20" s="53">
-        <f t="shared" ref="H20:L20" si="0">H13*-1</f>
+        <f t="shared" ref="H20:L20" si="2">H13*-1</f>
         <v>-1</v>
       </c>
       <c r="I20" s="53">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>-3</v>
       </c>
       <c r="J20" s="53">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K20" s="53">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="L20" s="54">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>-22</v>
       </c>
     </row>
@@ -2323,27 +4582,27 @@
         <v>5</v>
       </c>
       <c r="G24" s="47">
-        <f t="shared" ref="G24:L24" si="1">G17-$F24*G$27</f>
+        <f t="shared" ref="G24:L24" si="3">G17-$F24*G$27</f>
         <v>4.3333333333333339</v>
       </c>
       <c r="H24" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>2.3333333333333335</v>
       </c>
       <c r="I24" s="55">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="J24" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K24" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1.6666666666666665</v>
       </c>
       <c r="L24" s="48">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>-36.666666666666664</v>
       </c>
     </row>
@@ -2352,27 +4611,27 @@
         <v>4</v>
       </c>
       <c r="G25" s="24">
-        <f t="shared" ref="G25:L25" si="2">G18-$F25*G$27</f>
+        <f t="shared" ref="G25:L25" si="4">G18-$F25*G$27</f>
         <v>0.66666666666666674</v>
       </c>
       <c r="H25" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>-2.333333333333333</v>
       </c>
       <c r="I25" s="56">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="J25" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="K25" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1.3333333333333333</v>
       </c>
       <c r="L25" s="49">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>-9.3333333333333321</v>
       </c>
     </row>
@@ -2385,23 +4644,23 @@
         <v>1.3333333333333335</v>
       </c>
       <c r="H26" s="3">
-        <f t="shared" ref="H26:L26" si="3">H19-$F26*H$27</f>
+        <f t="shared" ref="H26:L26" si="5">H19-$F26*H$27</f>
         <v>5.333333333333333</v>
       </c>
       <c r="I26" s="56">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="J26" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="K26" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.66666666666666663</v>
       </c>
       <c r="L26" s="49">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>45.333333333333336</v>
       </c>
     </row>
@@ -2414,23 +4673,23 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="H27" s="53">
-        <f t="shared" ref="H27:L27" si="4">H20/$F27</f>
+        <f t="shared" ref="H27:L27" si="6">H20/$F27</f>
         <v>0.33333333333333331</v>
       </c>
       <c r="I27" s="53">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="J27" s="53">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="K27" s="53">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>-0.33333333333333331</v>
       </c>
       <c r="L27" s="54">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>7.333333333333333</v>
       </c>
     </row>
@@ -2576,27 +4835,27 @@
         <v>2.3333333333333335</v>
       </c>
       <c r="G38" s="57">
-        <f t="shared" ref="G38:L38" si="5">G31-$F38*G$39</f>
+        <f t="shared" ref="G38:L38" si="7">G31-$F38*G$39</f>
         <v>5.0000000000000009</v>
       </c>
       <c r="H38" s="55">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="I38" s="30">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="J38" s="30">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1.0000000000000002</v>
       </c>
       <c r="K38" s="30">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>3</v>
       </c>
       <c r="L38" s="31">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>-46</v>
       </c>
     </row>
@@ -2609,23 +4868,23 @@
         <v>-0.28571428571428581</v>
       </c>
       <c r="H39" s="56">
-        <f t="shared" ref="H39:L39" si="6">H32/$F39</f>
+        <f t="shared" ref="H39:L39" si="8">H32/$F39</f>
         <v>1</v>
       </c>
       <c r="I39" s="56">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="J39" s="56">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>-0.4285714285714286</v>
       </c>
       <c r="K39" s="56">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>-0.57142857142857151</v>
       </c>
       <c r="L39" s="62">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>4</v>
       </c>
     </row>
@@ -2634,27 +4893,27 @@
         <v>5.333333333333333</v>
       </c>
       <c r="G40" s="58">
-        <f t="shared" ref="G40:L40" si="7">G33-$F40*G$39</f>
+        <f t="shared" ref="G40:L40" si="9">G33-$F40*G$39</f>
         <v>2.8571428571428577</v>
       </c>
       <c r="H40" s="56">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="I40" s="21">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="J40" s="21">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>2.2857142857142856</v>
       </c>
       <c r="K40" s="21">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>3.7142857142857144</v>
       </c>
       <c r="L40" s="22">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>24.000000000000004</v>
       </c>
     </row>
@@ -2667,23 +4926,23 @@
         <v>0.4285714285714286</v>
       </c>
       <c r="H41" s="53">
-        <f t="shared" ref="H41:L41" si="8">H34-$F41*H$39</f>
+        <f t="shared" ref="H41:L41" si="10">H34-$F41*H$39</f>
         <v>0</v>
       </c>
       <c r="I41" s="60">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="J41" s="60">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0.14285714285714285</v>
       </c>
       <c r="K41" s="60">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>-0.14285714285714282</v>
       </c>
       <c r="L41" s="23">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
finalizado modelo 1 do trabalho 2
</commit_message>
<xml_diff>
--- a/trabalho02/rascunho.xlsx
+++ b/trabalho02/rascunho.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/acsjunior/Documents/Projects/ppgmne-mnum7078/trabalho02/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84E78CD0-27BB-2146-88D8-071A10E4B03F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5348D1F-7A77-D84A-8065-C4198C5A7635}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16940" activeTab="1" xr2:uid="{8808CF02-2367-564A-820C-A633E855AC6A}"/>
   </bookViews>
@@ -21,7 +21,7 @@
   </sheets>
   <definedNames>
     <definedName name="solver_adj" localSheetId="0" hidden="1">Sheet1!$J$8:$M$11,Sheet1!$J$13:$M$16,Sheet1!#REF!,Sheet1!#REF!</definedName>
-    <definedName name="solver_adj" localSheetId="1" hidden="1">'Sheet1 (2)'!$P$8:$S$11,'Sheet1 (2)'!$P$17:$S$17,'Sheet1 (2)'!$P$20:$S$23,'Sheet1 (2)'!$P$35:$S$35,'Sheet1 (2)'!$P$41:$S$44,'Sheet1 (2)'!$P$50:$S$50,'Sheet1 (2)'!$P$53:$S$56,'Sheet1 (2)'!$P$68:$S$68</definedName>
+    <definedName name="solver_adj" localSheetId="1" hidden="1">'Sheet1 (2)'!$O$8:$R$11,'Sheet1 (2)'!$O$19:$R$22,'Sheet1 (2)'!$O$26:$R$26,'Sheet1 (2)'!$O$33:$R$36,'Sheet1 (2)'!$O$42:$R$42</definedName>
     <definedName name="solver_adj" localSheetId="4" hidden="1">Sheet2!$AJ$10:$AN$10</definedName>
     <definedName name="solver_cvg" localSheetId="0" hidden="1">0.0001</definedName>
     <definedName name="solver_cvg" localSheetId="1" hidden="1">0.0001</definedName>
@@ -36,26 +36,26 @@
     <definedName name="solver_itr" localSheetId="1" hidden="1">2147483647</definedName>
     <definedName name="solver_itr" localSheetId="4" hidden="1">2147483647</definedName>
     <definedName name="solver_lhs1" localSheetId="0" hidden="1">Sheet1!$J$17:$M$17</definedName>
-    <definedName name="solver_lhs1" localSheetId="1" hidden="1">'Sheet1 (2)'!$P$14:$S$14</definedName>
+    <definedName name="solver_lhs1" localSheetId="1" hidden="1">'Sheet1 (2)'!$O$14:$R$14</definedName>
     <definedName name="solver_lhs1" localSheetId="4" hidden="1">Sheet2!$AO$12</definedName>
-    <definedName name="solver_lhs10" localSheetId="1" hidden="1">'Sheet1 (2)'!$P$65</definedName>
-    <definedName name="solver_lhs11" localSheetId="1" hidden="1">'Sheet1 (2)'!$P$68:$S$68</definedName>
-    <definedName name="solver_lhs12" localSheetId="1" hidden="1">'Sheet1 (2)'!$T$41:$T$44</definedName>
-    <definedName name="solver_lhs13" localSheetId="1" hidden="1">'Sheet1 (2)'!$T$8:$T$11</definedName>
+    <definedName name="solver_lhs10" localSheetId="1" hidden="1">'Sheet1 (2)'!#REF!</definedName>
+    <definedName name="solver_lhs11" localSheetId="1" hidden="1">'Sheet1 (2)'!#REF!</definedName>
+    <definedName name="solver_lhs12" localSheetId="1" hidden="1">'Sheet1 (2)'!#REF!</definedName>
+    <definedName name="solver_lhs13" localSheetId="1" hidden="1">'Sheet1 (2)'!#REF!</definedName>
     <definedName name="solver_lhs2" localSheetId="0" hidden="1">Sheet1!#REF!</definedName>
-    <definedName name="solver_lhs2" localSheetId="1" hidden="1">'Sheet1 (2)'!$P$17:$S$17</definedName>
+    <definedName name="solver_lhs2" localSheetId="1" hidden="1">'Sheet1 (2)'!$O$26:$R$26</definedName>
     <definedName name="solver_lhs2" localSheetId="4" hidden="1">Sheet2!$AO$13</definedName>
     <definedName name="solver_lhs3" localSheetId="0" hidden="1">Sheet1!#REF!</definedName>
-    <definedName name="solver_lhs3" localSheetId="1" hidden="1">'Sheet1 (2)'!$P$17:$S$17</definedName>
+    <definedName name="solver_lhs3" localSheetId="1" hidden="1">'Sheet1 (2)'!$O$26:$R$26</definedName>
     <definedName name="solver_lhs3" localSheetId="4" hidden="1">Sheet2!$AO$14</definedName>
     <definedName name="solver_lhs4" localSheetId="0" hidden="1">Sheet1!$N$8:$N$11</definedName>
-    <definedName name="solver_lhs4" localSheetId="1" hidden="1">'Sheet1 (2)'!$P$32</definedName>
+    <definedName name="solver_lhs4" localSheetId="1" hidden="1">'Sheet1 (2)'!$O$29:$R$29</definedName>
     <definedName name="solver_lhs5" localSheetId="0" hidden="1">Sheet1!#REF!</definedName>
-    <definedName name="solver_lhs5" localSheetId="1" hidden="1">'Sheet1 (2)'!$P$35:$S$35</definedName>
-    <definedName name="solver_lhs6" localSheetId="1" hidden="1">'Sheet1 (2)'!$P$36</definedName>
-    <definedName name="solver_lhs7" localSheetId="1" hidden="1">'Sheet1 (2)'!$P$47:$S$47</definedName>
-    <definedName name="solver_lhs8" localSheetId="1" hidden="1">'Sheet1 (2)'!$P$50:$S$50</definedName>
-    <definedName name="solver_lhs9" localSheetId="1" hidden="1">'Sheet1 (2)'!$P$50:$S$50</definedName>
+    <definedName name="solver_lhs5" localSheetId="1" hidden="1">'Sheet1 (2)'!$O$42:$R$42</definedName>
+    <definedName name="solver_lhs6" localSheetId="1" hidden="1">'Sheet1 (2)'!$S$42</definedName>
+    <definedName name="solver_lhs7" localSheetId="1" hidden="1">'Sheet1 (2)'!$S$8:$S$11</definedName>
+    <definedName name="solver_lhs8" localSheetId="1" hidden="1">'Sheet1 (2)'!#REF!</definedName>
+    <definedName name="solver_lhs9" localSheetId="1" hidden="1">'Sheet1 (2)'!#REF!</definedName>
     <definedName name="solver_lin" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_lin" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_lin" localSheetId="4" hidden="1">1</definedName>
@@ -78,10 +78,10 @@
     <definedName name="solver_nod" localSheetId="1" hidden="1">2147483647</definedName>
     <definedName name="solver_nod" localSheetId="4" hidden="1">2147483647</definedName>
     <definedName name="solver_num" localSheetId="0" hidden="1">4</definedName>
-    <definedName name="solver_num" localSheetId="1" hidden="1">13</definedName>
+    <definedName name="solver_num" localSheetId="1" hidden="1">7</definedName>
     <definedName name="solver_num" localSheetId="4" hidden="1">3</definedName>
     <definedName name="solver_opt" localSheetId="0" hidden="1">Sheet1!$J$3</definedName>
-    <definedName name="solver_opt" localSheetId="1" hidden="1">'Sheet1 (2)'!$P$3</definedName>
+    <definedName name="solver_opt" localSheetId="1" hidden="1">'Sheet1 (2)'!$O$2</definedName>
     <definedName name="solver_opt" localSheetId="4" hidden="1">Sheet2!$AO$11</definedName>
     <definedName name="solver_pre" localSheetId="0" hidden="1">0.000001</definedName>
     <definedName name="solver_pre" localSheetId="1" hidden="1">0.000001</definedName>
@@ -103,7 +103,7 @@
     <definedName name="solver_rel3" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_rel3" localSheetId="4" hidden="1">3</definedName>
     <definedName name="solver_rel4" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_rel4" localSheetId="1" hidden="1">3</definedName>
+    <definedName name="solver_rel4" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_rel5" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_rel5" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_rel6" localSheetId="1" hidden="1">2</definedName>
@@ -111,26 +111,26 @@
     <definedName name="solver_rel8" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_rel9" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_rhs1" localSheetId="0" hidden="1">Sheet1!$J$18:$M$18</definedName>
-    <definedName name="solver_rhs1" localSheetId="1" hidden="1">'Sheet1 (2)'!$P$13:$S$13</definedName>
+    <definedName name="solver_rhs1" localSheetId="1" hidden="1">'Sheet1 (2)'!$O$15:$R$15</definedName>
     <definedName name="solver_rhs1" localSheetId="4" hidden="1">Sheet2!$AR$12</definedName>
-    <definedName name="solver_rhs10" localSheetId="1" hidden="1">'Sheet1 (2)'!$P$66</definedName>
-    <definedName name="solver_rhs11" localSheetId="1" hidden="1">'Sheet1 (2)'!$P$62:$S$62</definedName>
-    <definedName name="solver_rhs12" localSheetId="1" hidden="1">'Sheet1 (2)'!$U$41:$U$44</definedName>
-    <definedName name="solver_rhs13" localSheetId="1" hidden="1">'Sheet1 (2)'!$U$8:$U$11</definedName>
+    <definedName name="solver_rhs10" localSheetId="1" hidden="1">'Sheet1 (2)'!#REF!</definedName>
+    <definedName name="solver_rhs11" localSheetId="1" hidden="1">'Sheet1 (2)'!#REF!</definedName>
+    <definedName name="solver_rhs12" localSheetId="1" hidden="1">'Sheet1 (2)'!#REF!</definedName>
+    <definedName name="solver_rhs13" localSheetId="1" hidden="1">'Sheet1 (2)'!#REF!</definedName>
     <definedName name="solver_rhs2" localSheetId="0" hidden="1">Sheet1!#REF!</definedName>
-    <definedName name="solver_rhs2" localSheetId="1" hidden="1">'Sheet1 (2)'!$P$14:$S$14</definedName>
+    <definedName name="solver_rhs2" localSheetId="1" hidden="1">'Sheet1 (2)'!$O$14:$R$14</definedName>
     <definedName name="solver_rhs2" localSheetId="4" hidden="1">Sheet2!$AR$13</definedName>
     <definedName name="solver_rhs3" localSheetId="0" hidden="1">Sheet1!#REF!</definedName>
-    <definedName name="solver_rhs3" localSheetId="1" hidden="1">'Sheet1 (2)'!$P$16:$S$16</definedName>
+    <definedName name="solver_rhs3" localSheetId="1" hidden="1">'Sheet1 (2)'!$O$27:$R$27</definedName>
     <definedName name="solver_rhs3" localSheetId="4" hidden="1">Sheet2!$AR$14</definedName>
     <definedName name="solver_rhs4" localSheetId="0" hidden="1">Sheet1!$O$8:$O$11</definedName>
-    <definedName name="solver_rhs4" localSheetId="1" hidden="1">'Sheet1 (2)'!$P$33</definedName>
+    <definedName name="solver_rhs4" localSheetId="1" hidden="1">'Sheet1 (2)'!$O$30:$R$30</definedName>
     <definedName name="solver_rhs5" localSheetId="0" hidden="1">Sheet1!#REF!</definedName>
-    <definedName name="solver_rhs5" localSheetId="1" hidden="1">'Sheet1 (2)'!$P$29:$S$29</definedName>
-    <definedName name="solver_rhs6" localSheetId="1" hidden="1">'Sheet1 (2)'!$Q$66</definedName>
-    <definedName name="solver_rhs7" localSheetId="1" hidden="1">'Sheet1 (2)'!$P$46:$S$46</definedName>
-    <definedName name="solver_rhs8" localSheetId="1" hidden="1">'Sheet1 (2)'!$P$47:$S$47</definedName>
-    <definedName name="solver_rhs9" localSheetId="1" hidden="1">'Sheet1 (2)'!$P$49:$S$49</definedName>
+    <definedName name="solver_rhs5" localSheetId="1" hidden="1">'Sheet1 (2)'!$O$29:$R$29</definedName>
+    <definedName name="solver_rhs6" localSheetId="1" hidden="1">'Sheet1 (2)'!$S$41</definedName>
+    <definedName name="solver_rhs7" localSheetId="1" hidden="1">'Sheet1 (2)'!$T$8:$T$11</definedName>
+    <definedName name="solver_rhs8" localSheetId="1" hidden="1">'Sheet1 (2)'!#REF!</definedName>
+    <definedName name="solver_rhs9" localSheetId="1" hidden="1">'Sheet1 (2)'!#REF!</definedName>
     <definedName name="solver_rlx" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_rlx" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_rlx" localSheetId="4" hidden="1">2</definedName>
@@ -172,7 +172,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="69">
   <si>
     <t>Blumenau</t>
   </si>
@@ -297,21 +297,9 @@
     <t>&gt;=</t>
   </si>
   <si>
-    <t>u_f'ft</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>v_f't</t>
-  </si>
-  <si>
     <t>y_ft</t>
   </si>
   <si>
-    <t>v_ft</t>
-  </si>
-  <si>
     <t>f1</t>
   </si>
   <si>
@@ -327,51 +315,21 @@
     <t>e'</t>
   </si>
   <si>
-    <t>total</t>
-  </si>
-  <si>
-    <t>w'_ft</t>
-  </si>
-  <si>
-    <t>e_ft</t>
-  </si>
-  <si>
-    <t>demanda</t>
-  </si>
-  <si>
-    <t>custo</t>
-  </si>
-  <si>
     <t>CEb_f</t>
   </si>
   <si>
     <t>CEp_f</t>
   </si>
   <si>
-    <t>sum(e_ft)</t>
-  </si>
-  <si>
-    <t>e'_ft</t>
-  </si>
-  <si>
     <t>FO:</t>
   </si>
   <si>
-    <t>Ep_f</t>
-  </si>
-  <si>
     <t>B &lt;= A*A</t>
   </si>
   <si>
     <t>3 &lt;= 2*2</t>
   </si>
   <si>
-    <t>sum(e'_ft)</t>
-  </si>
-  <si>
-    <t>Saldo</t>
-  </si>
-  <si>
     <t>Prod. Total</t>
   </si>
   <si>
@@ -381,13 +339,46 @@
     <t>Dif</t>
   </si>
   <si>
-    <t>Prod. Acum</t>
-  </si>
-  <si>
-    <t>Prev. Acum</t>
-  </si>
-  <si>
-    <t>Dem. Ok</t>
+    <t>ER</t>
+  </si>
+  <si>
+    <t>Período</t>
+  </si>
+  <si>
+    <t>h_rft</t>
+  </si>
+  <si>
+    <t>eb_ft</t>
+  </si>
+  <si>
+    <t>ER_f</t>
+  </si>
+  <si>
+    <t>tb_f'ft</t>
+  </si>
+  <si>
+    <t>P_f</t>
+  </si>
+  <si>
+    <t>ef_ft</t>
+  </si>
+  <si>
+    <t>EF_ft</t>
+  </si>
+  <si>
+    <t>tf_f'ft</t>
+  </si>
+  <si>
+    <t>Demanda</t>
+  </si>
+  <si>
+    <t>ef'_ft</t>
+  </si>
+  <si>
+    <t>eb'_ft</t>
+  </si>
+  <si>
+    <t>EB_f</t>
   </si>
 </sst>
 </file>
@@ -411,7 +402,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -457,6 +448,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -642,7 +645,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="74">
+  <cellXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -857,10 +860,28 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2318,10 +2339,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C8D0DC1-1099-834F-A649-D4073562A5D6}">
-  <dimension ref="C2:W69"/>
+  <dimension ref="C2:T46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2330,32 +2351,36 @@
     <col min="7" max="7" width="10.83203125" style="1" customWidth="1"/>
     <col min="8" max="8" width="13.5" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13.5" style="1" customWidth="1"/>
-    <col min="10" max="23" width="10.83203125" style="1"/>
+    <col min="10" max="12" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:22" x14ac:dyDescent="0.2">
-      <c r="P2" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="3" spans="3:22" x14ac:dyDescent="0.2">
-      <c r="O3" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="P3" s="73">
-        <f>V11+V14+V17+V23+V30+V44+V47+V50+V56+V63</f>
-        <v>27180000</v>
-      </c>
-    </row>
-    <row r="6" spans="3:22" x14ac:dyDescent="0.2">
-      <c r="O6" s="11" t="s">
+    <row r="2" spans="3:20" x14ac:dyDescent="0.2">
+      <c r="N2" s="76" t="s">
+        <v>49</v>
+      </c>
+      <c r="O2" s="81">
+        <f>S12+S16+S23+S26+S37+S43</f>
+        <v>9614000</v>
+      </c>
+    </row>
+    <row r="4" spans="3:20" x14ac:dyDescent="0.2">
+      <c r="N4" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="O4" s="77"/>
+      <c r="P4" s="32"/>
+      <c r="Q4" s="32"/>
+      <c r="R4" s="33"/>
+    </row>
+    <row r="6" spans="3:20" x14ac:dyDescent="0.2">
+      <c r="N6" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="O6" s="73">
         <v>9</v>
       </c>
-      <c r="P6" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="3:22" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="3:20" x14ac:dyDescent="0.2">
       <c r="C7" s="16" t="s">
         <v>12</v>
       </c>
@@ -2371,29 +2396,29 @@
       <c r="G7" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="O7" s="16" t="s">
+      <c r="N7" s="16" t="s">
         <v>8</v>
       </c>
+      <c r="O7" s="17" t="s">
+        <v>0</v>
+      </c>
       <c r="P7" s="17" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q7" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="R7" s="17" t="s">
         <v>2</v>
       </c>
+      <c r="R7" s="18" t="s">
+        <v>3</v>
+      </c>
       <c r="S7" s="18" t="s">
-        <v>3</v>
-      </c>
-      <c r="T7" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="U7" s="16" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="3:22" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+      <c r="T7" s="18" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="8" spans="3:20" x14ac:dyDescent="0.2">
       <c r="C8" s="19" t="s">
         <v>4</v>
       </c>
@@ -2409,31 +2434,31 @@
       <c r="G8" s="35">
         <v>26</v>
       </c>
-      <c r="O8" s="19" t="s">
+      <c r="N8" s="19" t="s">
         <v>4</v>
       </c>
+      <c r="O8" s="21">
+        <v>0</v>
+      </c>
       <c r="P8" s="21">
-        <v>16000</v>
+        <v>0</v>
       </c>
       <c r="Q8" s="21">
-        <v>0</v>
-      </c>
-      <c r="R8" s="21">
-        <v>194000</v>
-      </c>
-      <c r="S8" s="64">
-        <v>0</v>
-      </c>
-      <c r="T8" s="70">
-        <f>SUM(P8:S8)</f>
-        <v>210000</v>
-      </c>
-      <c r="U8" s="68">
-        <f>VLOOKUP(P6,$C$25:$G$37,2,0)</f>
-        <v>230000</v>
-      </c>
-    </row>
-    <row r="9" spans="3:22" x14ac:dyDescent="0.2">
+        <v>160000</v>
+      </c>
+      <c r="R8" s="64">
+        <v>0</v>
+      </c>
+      <c r="S8" s="70">
+        <f>SUM(O8:R8)</f>
+        <v>160000</v>
+      </c>
+      <c r="T8" s="74">
+        <f>VLOOKUP(O6,$C$25:$G$37,2,0)</f>
+        <v>260000</v>
+      </c>
+    </row>
+    <row r="9" spans="3:20" x14ac:dyDescent="0.2">
       <c r="C9" s="19" t="s">
         <v>5</v>
       </c>
@@ -2449,31 +2474,31 @@
       <c r="G9" s="35">
         <v>25.2</v>
       </c>
-      <c r="O9" s="19" t="s">
+      <c r="N9" s="19" t="s">
         <v>5</v>
       </c>
+      <c r="O9" s="21">
+        <v>240000</v>
+      </c>
       <c r="P9" s="21">
-        <v>8000</v>
+        <v>140000</v>
       </c>
       <c r="Q9" s="21">
-        <v>112000</v>
-      </c>
-      <c r="R9" s="21">
-        <v>0</v>
-      </c>
-      <c r="S9" s="64">
-        <v>0</v>
-      </c>
-      <c r="T9" s="43">
-        <f t="shared" ref="T9:T11" si="0">SUM(P9:S9)</f>
-        <v>120000</v>
-      </c>
-      <c r="U9" s="68">
-        <f>VLOOKUP(P6,$C$25:$G$37,3,0)</f>
-        <v>120000</v>
-      </c>
-    </row>
-    <row r="10" spans="3:22" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="R9" s="64">
+        <v>0</v>
+      </c>
+      <c r="S9" s="43">
+        <f t="shared" ref="S9:S11" si="0">SUM(O9:R9)</f>
+        <v>380000</v>
+      </c>
+      <c r="T9" s="68">
+        <f>VLOOKUP(O6,$C$25:$G$37,3,0)</f>
+        <v>380000</v>
+      </c>
+    </row>
+    <row r="10" spans="3:20" x14ac:dyDescent="0.2">
       <c r="C10" s="19" t="s">
         <v>6</v>
       </c>
@@ -2489,34 +2514,31 @@
       <c r="G10" s="35">
         <v>21.6</v>
       </c>
-      <c r="O10" s="19" t="s">
+      <c r="N10" s="19" t="s">
         <v>6</v>
       </c>
+      <c r="O10" s="21">
+        <v>0</v>
+      </c>
       <c r="P10" s="21">
         <v>0</v>
       </c>
       <c r="Q10" s="21">
-        <v>74000</v>
-      </c>
-      <c r="R10" s="21">
-        <v>0</v>
-      </c>
-      <c r="S10" s="64">
-        <v>136000</v>
-      </c>
-      <c r="T10" s="43">
+        <v>0</v>
+      </c>
+      <c r="R10" s="64">
+        <v>0</v>
+      </c>
+      <c r="S10" s="43">
         <f t="shared" si="0"/>
-        <v>210000</v>
-      </c>
-      <c r="U10" s="68">
-        <f>VLOOKUP(P6,$C$25:$G$37,4,0)</f>
-        <v>210000</v>
-      </c>
-      <c r="V10" s="16" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="11" spans="3:22" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="T10" s="68">
+        <f>VLOOKUP(O6,$C$25:$G$37,4,0)</f>
+        <v>370000</v>
+      </c>
+    </row>
+    <row r="11" spans="3:20" x14ac:dyDescent="0.2">
       <c r="C11" s="20" t="s">
         <v>7</v>
       </c>
@@ -2532,35 +2554,56 @@
       <c r="G11" s="37">
         <v>10.8</v>
       </c>
-      <c r="O11" s="20" t="s">
+      <c r="N11" s="20" t="s">
         <v>7</v>
       </c>
+      <c r="O11" s="60">
+        <v>0</v>
+      </c>
       <c r="P11" s="60">
         <v>0</v>
       </c>
       <c r="Q11" s="60">
         <v>0</v>
       </c>
-      <c r="R11" s="60">
-        <v>0</v>
-      </c>
-      <c r="S11" s="65">
-        <v>0</v>
-      </c>
-      <c r="T11" s="44">
+      <c r="R11" s="65">
+        <v>60000</v>
+      </c>
+      <c r="S11" s="44">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="U11" s="69">
-        <f>VLOOKUP(P6,$C$25:$G$37,5,0)</f>
-        <v>0</v>
-      </c>
-      <c r="V11" s="71">
-        <f>SUMPRODUCT($D$8:$G$11,P8:S11)</f>
-        <v>5664800</v>
-      </c>
-    </row>
-    <row r="13" spans="3:22" x14ac:dyDescent="0.2">
+        <v>60000</v>
+      </c>
+      <c r="T11" s="69">
+        <f>VLOOKUP(O6,$C$25:$G$37,5,0)</f>
+        <v>260000</v>
+      </c>
+    </row>
+    <row r="12" spans="3:20" x14ac:dyDescent="0.2">
+      <c r="N12" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="O12" s="13">
+        <f>SUM(O8:O11)</f>
+        <v>240000</v>
+      </c>
+      <c r="P12" s="13">
+        <f t="shared" ref="P12:R12" si="1">SUM(P8:P11)</f>
+        <v>140000</v>
+      </c>
+      <c r="Q12" s="13">
+        <f t="shared" si="1"/>
+        <v>160000</v>
+      </c>
+      <c r="R12" s="14">
+        <f t="shared" si="1"/>
+        <v>60000</v>
+      </c>
+      <c r="S12" s="81">
+        <f>SUMPRODUCT($D$8:$G$11,O8:R11)</f>
+        <v>3224000</v>
+      </c>
+    </row>
+    <row r="13" spans="3:20" x14ac:dyDescent="0.2">
       <c r="C13" s="16" t="s">
         <v>17</v>
       </c>
@@ -2576,26 +2619,8 @@
       <c r="G13" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="O13" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="P13" s="32">
-        <v>1500000</v>
-      </c>
-      <c r="Q13" s="32">
-        <v>750000</v>
-      </c>
-      <c r="R13" s="32">
-        <v>1250000</v>
-      </c>
-      <c r="S13" s="33">
-        <v>1000000</v>
-      </c>
-      <c r="V13" s="16" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="14" spans="3:22" x14ac:dyDescent="0.2">
+    </row>
+    <row r="14" spans="3:20" x14ac:dyDescent="0.2">
       <c r="C14" s="19" t="s">
         <v>0</v>
       </c>
@@ -2611,31 +2636,27 @@
       <c r="G14" s="35">
         <v>18.399999999999999</v>
       </c>
-      <c r="O14" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="P14" s="13">
-        <f>SUM(P8:P11)</f>
-        <v>24000</v>
-      </c>
-      <c r="Q14" s="13">
-        <f t="shared" ref="Q14:S14" si="1">SUM(Q8:Q11)</f>
-        <v>186000</v>
-      </c>
-      <c r="R14" s="13">
-        <f t="shared" si="1"/>
-        <v>194000</v>
-      </c>
-      <c r="S14" s="14">
-        <f t="shared" si="1"/>
-        <v>136000</v>
-      </c>
-      <c r="V14" s="71">
-        <f>SUMPRODUCT($D$19:$G$19,P14:S14)</f>
-        <v>3742400</v>
-      </c>
-    </row>
-    <row r="15" spans="3:22" x14ac:dyDescent="0.2">
+      <c r="N14" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="O14" s="78">
+        <f>O4+O12+O23-O24</f>
+        <v>240000</v>
+      </c>
+      <c r="P14" s="78">
+        <f>P4+P12+P23-P24</f>
+        <v>140000</v>
+      </c>
+      <c r="Q14" s="78">
+        <f>Q4+Q12+Q23-Q24</f>
+        <v>160000</v>
+      </c>
+      <c r="R14" s="79">
+        <f>R4+R12+R23-R24</f>
+        <v>60000</v>
+      </c>
+    </row>
+    <row r="15" spans="3:20" x14ac:dyDescent="0.2">
       <c r="C15" s="19" t="s">
         <v>1</v>
       </c>
@@ -2651,8 +2672,23 @@
       <c r="G15" s="35">
         <v>17.2</v>
       </c>
-    </row>
-    <row r="16" spans="3:22" x14ac:dyDescent="0.2">
+      <c r="N15" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="O15" s="32">
+        <v>1500000</v>
+      </c>
+      <c r="P15" s="32">
+        <v>750000</v>
+      </c>
+      <c r="Q15" s="32">
+        <v>1250000</v>
+      </c>
+      <c r="R15" s="33">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="16" spans="3:20" x14ac:dyDescent="0.2">
       <c r="C16" s="19" t="s">
         <v>2</v>
       </c>
@@ -2668,26 +2704,31 @@
       <c r="G16" s="35">
         <v>22.8</v>
       </c>
-      <c r="O16" s="46" t="s">
-        <v>25</v>
-      </c>
-      <c r="P16" s="32">
-        <v>24000</v>
-      </c>
-      <c r="Q16" s="32">
-        <v>180000</v>
-      </c>
-      <c r="R16" s="32">
-        <v>160000</v>
-      </c>
-      <c r="S16" s="33">
-        <v>170000</v>
-      </c>
-      <c r="V16" s="16" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="17" spans="3:22" x14ac:dyDescent="0.2">
+      <c r="N16" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="O16" s="78">
+        <f>O14-O26</f>
+        <v>0</v>
+      </c>
+      <c r="P16" s="78">
+        <f t="shared" ref="P16:R16" si="2">P14-P26</f>
+        <v>0</v>
+      </c>
+      <c r="Q16" s="78">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="R16" s="79">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="S16" s="81">
+        <f>SUMPRODUCT($D$19:$G$19,O16:R16)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="3:19" x14ac:dyDescent="0.2">
       <c r="C17" s="20" t="s">
         <v>3</v>
       </c>
@@ -2703,29 +2744,30 @@
       <c r="G17" s="37">
         <v>0</v>
       </c>
-      <c r="O17" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="P17" s="30">
-        <v>24000</v>
-      </c>
-      <c r="Q17" s="30">
-        <v>116000</v>
-      </c>
-      <c r="R17" s="30">
-        <v>160000</v>
-      </c>
-      <c r="S17" s="67">
-        <v>0</v>
-      </c>
-      <c r="V17" s="71">
-        <f>SUMPRODUCT($D$21:$G$21,P17:S17)</f>
-        <v>3237600</v>
-      </c>
-    </row>
-    <row r="19" spans="3:22" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="3:19" x14ac:dyDescent="0.2">
+      <c r="N18" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="O18" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="P18" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q18" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="R18" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="S18" s="16" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="3:19" x14ac:dyDescent="0.2">
       <c r="C19" s="16" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="D19" s="32">
         <v>8.1</v>
@@ -2739,27 +2781,31 @@
       <c r="G19" s="33">
         <v>5.4</v>
       </c>
-      <c r="O19" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="P19" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q19" s="17" t="s">
+      <c r="N19" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="O19" s="21">
+        <v>0</v>
+      </c>
+      <c r="P19" s="21">
+        <v>0</v>
+      </c>
+      <c r="Q19" s="21">
+        <v>0</v>
+      </c>
+      <c r="R19" s="64">
+        <v>0</v>
+      </c>
+      <c r="S19" s="43">
+        <f>SUM(O19:R19)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="3:19" x14ac:dyDescent="0.2">
+      <c r="N20" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="R19" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="S19" s="18" t="s">
-        <v>3</v>
-      </c>
-      <c r="T19" s="16" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="20" spans="3:22" x14ac:dyDescent="0.2">
-      <c r="O20" s="19" t="s">
+      <c r="O20" s="21">
         <v>0</v>
       </c>
       <c r="P20" s="21">
@@ -2768,18 +2814,15 @@
       <c r="Q20" s="21">
         <v>0</v>
       </c>
-      <c r="R20" s="21">
-        <v>0</v>
-      </c>
-      <c r="S20" s="64">
-        <v>0</v>
-      </c>
-      <c r="T20" s="43">
-        <f>SUM(P20:S20)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="3:22" x14ac:dyDescent="0.2">
+      <c r="R20" s="64">
+        <v>0</v>
+      </c>
+      <c r="S20" s="43">
+        <f t="shared" ref="S20:S22" si="3">SUM(O20:R20)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="3:19" x14ac:dyDescent="0.2">
       <c r="C21" s="46" t="s">
         <v>23</v>
       </c>
@@ -2795,8 +2838,11 @@
       <c r="G21" s="33">
         <v>10.5</v>
       </c>
-      <c r="O21" s="19" t="s">
-        <v>1</v>
+      <c r="N21" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="O21" s="21">
+        <v>0</v>
       </c>
       <c r="P21" s="21">
         <v>0</v>
@@ -2804,44 +2850,38 @@
       <c r="Q21" s="21">
         <v>0</v>
       </c>
-      <c r="R21" s="21">
-        <v>0</v>
-      </c>
-      <c r="S21" s="64">
-        <v>0</v>
-      </c>
-      <c r="T21" s="43">
-        <f t="shared" ref="T21:T23" si="2">SUM(P21:S21)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="3:22" x14ac:dyDescent="0.2">
-      <c r="O22" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="P22" s="21">
-        <v>0</v>
-      </c>
-      <c r="Q22" s="21">
-        <v>0</v>
-      </c>
-      <c r="R22" s="21">
-        <v>0</v>
-      </c>
-      <c r="S22" s="64">
-        <v>0</v>
-      </c>
-      <c r="T22" s="43">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="V22" s="16" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="23" spans="3:22" x14ac:dyDescent="0.2">
+      <c r="R21" s="64">
+        <v>0</v>
+      </c>
+      <c r="S21" s="43">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="3:19" x14ac:dyDescent="0.2">
+      <c r="N22" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="O22" s="60">
+        <v>0</v>
+      </c>
+      <c r="P22" s="60">
+        <v>0</v>
+      </c>
+      <c r="Q22" s="60">
+        <v>0</v>
+      </c>
+      <c r="R22" s="65">
+        <v>0</v>
+      </c>
+      <c r="S22" s="44">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="3:19" x14ac:dyDescent="0.2">
       <c r="C23" s="16" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="D23" s="32">
         <v>5.3</v>
@@ -2855,31 +2895,50 @@
       <c r="G23" s="33">
         <v>3.8</v>
       </c>
-      <c r="O23" s="20" t="s">
-        <v>3</v>
-      </c>
-      <c r="P23" s="60">
-        <v>0</v>
-      </c>
-      <c r="Q23" s="60">
-        <v>0</v>
-      </c>
-      <c r="R23" s="60">
-        <v>0</v>
-      </c>
-      <c r="S23" s="65">
-        <v>0</v>
-      </c>
-      <c r="T23" s="44">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="V23" s="71">
-        <f>SUMPRODUCT($D$14:$G$17,P20:S23)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="3:22" x14ac:dyDescent="0.2">
+      <c r="N23" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="O23" s="13">
+        <f>SUM(O19:O22)</f>
+        <v>0</v>
+      </c>
+      <c r="P23" s="13">
+        <f t="shared" ref="P23:R23" si="4">SUM(P19:P22)</f>
+        <v>0</v>
+      </c>
+      <c r="Q23" s="13">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="R23" s="14">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="S23" s="81">
+        <f>SUMPRODUCT($D$14:$G$17,O19:R22)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="3:19" x14ac:dyDescent="0.2">
+      <c r="N24" s="75"/>
+      <c r="O24" s="13">
+        <f>S19</f>
+        <v>0</v>
+      </c>
+      <c r="P24" s="13">
+        <f>S20</f>
+        <v>0</v>
+      </c>
+      <c r="Q24" s="13">
+        <f>S21</f>
+        <v>0</v>
+      </c>
+      <c r="R24" s="14">
+        <f>S22</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="3:19" x14ac:dyDescent="0.2">
       <c r="C25" s="16" t="s">
         <v>19</v>
       </c>
@@ -2896,44 +2955,16 @@
         <v>7</v>
       </c>
       <c r="H25" s="66" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="I25" s="17" t="s">
-        <v>67</v>
+        <v>53</v>
       </c>
       <c r="J25" s="17" t="s">
-        <v>69</v>
-      </c>
-      <c r="K25" s="17" t="s">
-        <v>70</v>
-      </c>
-      <c r="L25" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="M25" s="18" t="s">
-        <v>71</v>
-      </c>
-      <c r="O25" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="P25" s="13">
-        <f>T20</f>
-        <v>0</v>
-      </c>
-      <c r="Q25" s="13">
-        <f>T21</f>
-        <v>0</v>
-      </c>
-      <c r="R25" s="13">
-        <f>T22</f>
-        <v>0</v>
-      </c>
-      <c r="S25" s="14">
-        <f>T23</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="3:22" x14ac:dyDescent="0.2">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="26" spans="3:19" x14ac:dyDescent="0.2">
       <c r="C26" s="19">
         <v>1</v>
       </c>
@@ -2957,23 +2988,30 @@
         <v>300000</v>
       </c>
       <c r="J26" s="1">
-        <f>H26</f>
-        <v>560000</v>
-      </c>
-      <c r="K26" s="1">
-        <f>I26</f>
-        <v>300000</v>
-      </c>
-      <c r="L26" s="1">
-        <f>J26-K26</f>
+        <f>H26-I26</f>
         <v>260000</v>
       </c>
-      <c r="M26" s="1">
-        <f>I26</f>
-        <v>300000</v>
-      </c>
-    </row>
-    <row r="27" spans="3:22" x14ac:dyDescent="0.2">
+      <c r="N26" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="O26" s="30">
+        <v>240000</v>
+      </c>
+      <c r="P26" s="30">
+        <v>140000</v>
+      </c>
+      <c r="Q26" s="30">
+        <v>160000</v>
+      </c>
+      <c r="R26" s="67">
+        <v>60000</v>
+      </c>
+      <c r="S26" s="81">
+        <f>SUMPRODUCT($D$21:$G$21,O26:R26)</f>
+        <v>6390000</v>
+      </c>
+    </row>
+    <row r="27" spans="3:19" x14ac:dyDescent="0.2">
       <c r="C27" s="19">
         <v>2</v>
       </c>
@@ -2990,49 +3028,33 @@
         <v>0</v>
       </c>
       <c r="H27" s="1">
-        <f t="shared" ref="H27:H37" si="3">SUM(D27:G27)</f>
+        <f t="shared" ref="H27:H37" si="5">SUM(D27:G27)</f>
         <v>260000</v>
       </c>
       <c r="I27" s="1">
         <v>500000</v>
       </c>
       <c r="J27" s="1">
-        <f>H27+J26</f>
-        <v>820000</v>
-      </c>
-      <c r="K27" s="1">
-        <f>I27+K26</f>
-        <v>800000</v>
-      </c>
-      <c r="L27" s="1">
-        <f>J27-K27</f>
-        <v>20000</v>
-      </c>
-      <c r="M27" s="1">
-        <f>I27</f>
-        <v>500000</v>
-      </c>
-      <c r="O27" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="P27" s="13">
-        <f>P14-P17-P25</f>
-        <v>0</v>
-      </c>
-      <c r="Q27" s="13">
-        <f>Q14-Q17-Q25</f>
-        <v>70000</v>
-      </c>
-      <c r="R27" s="13">
-        <f>R14-R17-R25</f>
-        <v>34000</v>
-      </c>
-      <c r="S27" s="14">
-        <f>S14-S17-S25</f>
-        <v>136000</v>
-      </c>
-    </row>
-    <row r="28" spans="3:22" x14ac:dyDescent="0.2">
+        <f>H27-I27</f>
+        <v>-240000</v>
+      </c>
+      <c r="N27" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="O27" s="32">
+        <v>240000</v>
+      </c>
+      <c r="P27" s="32">
+        <v>180000</v>
+      </c>
+      <c r="Q27" s="32">
+        <v>160000</v>
+      </c>
+      <c r="R27" s="33">
+        <v>170000</v>
+      </c>
+    </row>
+    <row r="28" spans="3:19" x14ac:dyDescent="0.2">
       <c r="C28" s="19">
         <v>3</v>
       </c>
@@ -3049,30 +3071,14 @@
         <v>0</v>
       </c>
       <c r="H28" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="I28" s="1">
         <v>700000</v>
       </c>
-      <c r="J28" s="1">
-        <f t="shared" ref="J28:J37" si="4">H28+J27</f>
-        <v>820000</v>
-      </c>
-      <c r="K28" s="1">
-        <f t="shared" ref="K28:K37" si="5">I28+K27</f>
-        <v>1500000</v>
-      </c>
-      <c r="L28" s="1">
-        <f>J28-K28</f>
-        <v>-680000</v>
-      </c>
-      <c r="M28" s="1">
-        <f>I28+L28</f>
-        <v>20000</v>
-      </c>
-    </row>
-    <row r="29" spans="3:22" x14ac:dyDescent="0.2">
+    </row>
+    <row r="29" spans="3:19" x14ac:dyDescent="0.2">
       <c r="C29" s="19">
         <v>4</v>
       </c>
@@ -3089,40 +3095,37 @@
         <v>0</v>
       </c>
       <c r="H29" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="I29" s="1">
         <v>900000</v>
       </c>
-      <c r="J29" s="1">
-        <f t="shared" si="4"/>
-        <v>820000</v>
-      </c>
-      <c r="K29" s="1">
-        <f t="shared" si="5"/>
-        <v>2400000</v>
-      </c>
-      <c r="O29" s="46" t="s">
-        <v>61</v>
-      </c>
-      <c r="P29" s="32">
-        <v>1000000</v>
-      </c>
-      <c r="Q29" s="32">
-        <v>800000</v>
-      </c>
-      <c r="R29" s="32">
-        <v>1000000</v>
-      </c>
-      <c r="S29" s="33">
-        <v>900000</v>
-      </c>
-      <c r="V29" s="16" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="30" spans="3:22" x14ac:dyDescent="0.2">
+      <c r="N29" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="O29" s="78">
+        <f>O26+O37-O38</f>
+        <v>240000</v>
+      </c>
+      <c r="P29" s="78">
+        <f t="shared" ref="P29:R29" si="6">P26+P37-P38</f>
+        <v>140000</v>
+      </c>
+      <c r="Q29" s="78">
+        <f t="shared" si="6"/>
+        <v>160000</v>
+      </c>
+      <c r="R29" s="79">
+        <f t="shared" si="6"/>
+        <v>60000</v>
+      </c>
+      <c r="S29" s="71">
+        <f>SUM(O29:R29)</f>
+        <v>600000</v>
+      </c>
+    </row>
+    <row r="30" spans="3:19" x14ac:dyDescent="0.2">
       <c r="C30" s="19">
         <v>5</v>
       </c>
@@ -3139,45 +3142,29 @@
         <v>100000</v>
       </c>
       <c r="H30" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>100000</v>
       </c>
       <c r="I30" s="1">
         <v>800000</v>
       </c>
-      <c r="J30" s="1">
-        <f t="shared" si="4"/>
-        <v>920000</v>
-      </c>
-      <c r="K30" s="1">
-        <f t="shared" si="5"/>
-        <v>3200000</v>
-      </c>
-      <c r="O30" s="16" t="s">
-        <v>53</v>
-      </c>
-      <c r="P30" s="13">
-        <f>P17</f>
-        <v>24000</v>
-      </c>
-      <c r="Q30" s="13">
-        <f>Q17</f>
-        <v>116000</v>
-      </c>
-      <c r="R30" s="13">
-        <f>R17</f>
-        <v>160000</v>
-      </c>
-      <c r="S30" s="14">
-        <f>S17</f>
-        <v>0</v>
-      </c>
-      <c r="V30" s="71">
-        <f>SUMPRODUCT($D$23:$G$23,P30:S30)</f>
-        <v>1338800</v>
-      </c>
-    </row>
-    <row r="31" spans="3:22" x14ac:dyDescent="0.2">
+      <c r="N30" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="O30" s="32">
+        <v>1000000</v>
+      </c>
+      <c r="P30" s="32">
+        <v>800000</v>
+      </c>
+      <c r="Q30" s="32">
+        <v>1000000</v>
+      </c>
+      <c r="R30" s="33">
+        <v>9000000</v>
+      </c>
+    </row>
+    <row r="31" spans="3:19" x14ac:dyDescent="0.2">
       <c r="C31" s="19">
         <v>6</v>
       </c>
@@ -3194,22 +3181,14 @@
         <v>110000</v>
       </c>
       <c r="H31" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>220000</v>
       </c>
       <c r="I31" s="1">
         <v>800000</v>
       </c>
-      <c r="J31" s="1">
-        <f t="shared" si="4"/>
-        <v>1140000</v>
-      </c>
-      <c r="K31" s="1">
-        <f t="shared" si="5"/>
-        <v>4000000</v>
-      </c>
-    </row>
-    <row r="32" spans="3:22" x14ac:dyDescent="0.2">
+    </row>
+    <row r="32" spans="3:19" x14ac:dyDescent="0.2">
       <c r="C32" s="19">
         <v>7</v>
       </c>
@@ -3226,32 +3205,36 @@
         <v>150000</v>
       </c>
       <c r="H32" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>670000</v>
       </c>
       <c r="I32" s="1">
         <v>700000</v>
       </c>
       <c r="J32" s="1">
-        <f t="shared" si="4"/>
-        <v>1810000</v>
-      </c>
-      <c r="K32" s="1">
-        <f t="shared" si="5"/>
-        <v>4700000</v>
-      </c>
-      <c r="O32" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="P32" s="71">
-        <f>SUM(P30:S30)</f>
-        <v>300000</v>
-      </c>
-      <c r="Q32" s="16" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="33" spans="3:22" x14ac:dyDescent="0.2">
+        <f>H32-I32</f>
+        <v>-30000</v>
+      </c>
+      <c r="N32" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="O32" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="P32" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q32" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="R32" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="S32" s="16" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="33" spans="3:19" x14ac:dyDescent="0.2">
       <c r="C33" s="19">
         <v>8</v>
       </c>
@@ -3268,32 +3251,37 @@
         <v>250000</v>
       </c>
       <c r="H33" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>1030000</v>
       </c>
       <c r="I33" s="1">
         <v>600000</v>
       </c>
-      <c r="J33" s="1">
-        <f t="shared" si="4"/>
-        <v>2840000</v>
-      </c>
-      <c r="K33" s="1">
-        <f t="shared" si="5"/>
-        <v>5300000</v>
-      </c>
-      <c r="O33" s="16" t="s">
-        <v>54</v>
-      </c>
-      <c r="P33" s="72">
-        <v>300000</v>
-      </c>
-      <c r="Q33" s="71">
-        <f>P32-P33</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="3:22" x14ac:dyDescent="0.2">
+      <c r="J33" s="72">
+        <f>H33-I33</f>
+        <v>430000</v>
+      </c>
+      <c r="N33" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="O33" s="21">
+        <v>0</v>
+      </c>
+      <c r="P33" s="21">
+        <v>0</v>
+      </c>
+      <c r="Q33" s="21">
+        <v>0</v>
+      </c>
+      <c r="R33" s="64">
+        <v>0</v>
+      </c>
+      <c r="S33" s="43">
+        <f>SUM(O33:R33)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="3:19" x14ac:dyDescent="0.2">
       <c r="C34" s="19">
         <v>9</v>
       </c>
@@ -3310,22 +3298,37 @@
         <v>260000</v>
       </c>
       <c r="H34" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>1270000</v>
       </c>
       <c r="I34" s="1">
         <v>600000</v>
       </c>
       <c r="J34" s="1">
-        <f t="shared" si="4"/>
-        <v>4110000</v>
-      </c>
-      <c r="K34" s="1">
-        <f t="shared" si="5"/>
-        <v>5900000</v>
-      </c>
-    </row>
-    <row r="35" spans="3:22" x14ac:dyDescent="0.2">
+        <f>H34-I34</f>
+        <v>670000</v>
+      </c>
+      <c r="N34" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="O34" s="21">
+        <v>0</v>
+      </c>
+      <c r="P34" s="21">
+        <v>0</v>
+      </c>
+      <c r="Q34" s="21">
+        <v>0</v>
+      </c>
+      <c r="R34" s="64">
+        <v>0</v>
+      </c>
+      <c r="S34" s="43">
+        <f t="shared" ref="S34:S36" si="7">SUM(O34:R34)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="3:19" x14ac:dyDescent="0.2">
       <c r="C35" s="19">
         <v>10</v>
       </c>
@@ -3342,37 +3345,33 @@
         <v>250000</v>
       </c>
       <c r="H35" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>1300000</v>
       </c>
       <c r="I35" s="1">
         <v>500000</v>
       </c>
-      <c r="J35" s="1">
-        <f t="shared" si="4"/>
-        <v>5410000</v>
-      </c>
-      <c r="K35" s="1">
-        <f t="shared" si="5"/>
-        <v>6400000</v>
-      </c>
-      <c r="O35" s="16" t="s">
-        <v>59</v>
-      </c>
-      <c r="P35" s="30">
-        <v>0</v>
-      </c>
-      <c r="Q35" s="30">
-        <v>0</v>
-      </c>
-      <c r="R35" s="30">
-        <v>0</v>
-      </c>
-      <c r="S35" s="67">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="3:22" x14ac:dyDescent="0.2">
+      <c r="N35" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="O35" s="21">
+        <v>0</v>
+      </c>
+      <c r="P35" s="21">
+        <v>0</v>
+      </c>
+      <c r="Q35" s="21">
+        <v>0</v>
+      </c>
+      <c r="R35" s="64">
+        <v>0</v>
+      </c>
+      <c r="S35" s="43">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="3:19" x14ac:dyDescent="0.2">
       <c r="C36" s="19">
         <v>11</v>
       </c>
@@ -3389,29 +3388,33 @@
         <v>200000</v>
       </c>
       <c r="H36" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>1350000</v>
       </c>
       <c r="I36" s="1">
         <v>500000</v>
       </c>
-      <c r="J36" s="1">
-        <f t="shared" si="4"/>
-        <v>6760000</v>
-      </c>
-      <c r="K36" s="1">
-        <f t="shared" si="5"/>
-        <v>6900000</v>
-      </c>
-      <c r="O36" s="16" t="s">
-        <v>64</v>
-      </c>
-      <c r="P36" s="71">
-        <f>SUM(P35:S35)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="3:22" x14ac:dyDescent="0.2">
+      <c r="N36" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="O36" s="60">
+        <v>0</v>
+      </c>
+      <c r="P36" s="60">
+        <v>0</v>
+      </c>
+      <c r="Q36" s="60">
+        <v>0</v>
+      </c>
+      <c r="R36" s="65">
+        <v>0</v>
+      </c>
+      <c r="S36" s="44">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="3:19" x14ac:dyDescent="0.2">
       <c r="C37" s="20">
         <v>12</v>
       </c>
@@ -3428,514 +3431,125 @@
         <v>120000</v>
       </c>
       <c r="H37" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>1080000</v>
       </c>
       <c r="I37" s="1">
         <v>400000</v>
       </c>
-      <c r="J37" s="1">
-        <f t="shared" si="4"/>
-        <v>7840000</v>
-      </c>
-      <c r="K37" s="1">
-        <f t="shared" si="5"/>
-        <v>7300000</v>
-      </c>
-    </row>
-    <row r="38" spans="3:22" x14ac:dyDescent="0.2">
+      <c r="N37" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="O37" s="13">
+        <f>SUM(O33:O36)</f>
+        <v>0</v>
+      </c>
+      <c r="P37" s="13">
+        <f t="shared" ref="P37" si="8">SUM(P33:P36)</f>
+        <v>0</v>
+      </c>
+      <c r="Q37" s="13">
+        <f t="shared" ref="Q37" si="9">SUM(Q33:Q36)</f>
+        <v>0</v>
+      </c>
+      <c r="R37" s="14">
+        <f t="shared" ref="R37" si="10">SUM(R33:R36)</f>
+        <v>0</v>
+      </c>
+      <c r="S37" s="81">
+        <f>SUMPRODUCT($D$14:$G$17,O33:R36)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="3:19" x14ac:dyDescent="0.2">
       <c r="F38"/>
       <c r="G38"/>
-    </row>
-    <row r="39" spans="3:22" x14ac:dyDescent="0.2">
+      <c r="N38" s="75"/>
+      <c r="O38" s="13">
+        <f>S33</f>
+        <v>0</v>
+      </c>
+      <c r="P38" s="13">
+        <f>S34</f>
+        <v>0</v>
+      </c>
+      <c r="Q38" s="13">
+        <f>S35</f>
+        <v>0</v>
+      </c>
+      <c r="R38" s="14">
+        <f>S36</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="3:19" x14ac:dyDescent="0.2">
+      <c r="C39" t="s">
+        <v>55</v>
+      </c>
       <c r="F39"/>
       <c r="G39"/>
-      <c r="O39" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="P39" s="12">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="40" spans="3:22" x14ac:dyDescent="0.2">
+    </row>
+    <row r="40" spans="3:19" x14ac:dyDescent="0.2">
       <c r="F40"/>
       <c r="G40"/>
-      <c r="O40" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="P40" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q40" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="R40" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="S40" s="18" t="s">
-        <v>3</v>
-      </c>
-      <c r="T40" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="U40" s="16" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="41" spans="3:22" x14ac:dyDescent="0.2">
+      <c r="N40" s="66" t="s">
+        <v>65</v>
+      </c>
+      <c r="O40" s="48">
+        <f>VLOOKUP(O6,$C$25:$I$37,7,0)</f>
+        <v>600000</v>
+      </c>
+    </row>
+    <row r="41" spans="3:19" x14ac:dyDescent="0.2">
       <c r="F41"/>
       <c r="G41"/>
-      <c r="O41" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="P41" s="21">
-        <v>24000</v>
-      </c>
-      <c r="Q41" s="21">
-        <v>0</v>
-      </c>
-      <c r="R41" s="21">
-        <v>126000</v>
-      </c>
-      <c r="S41" s="64">
-        <v>0</v>
-      </c>
-      <c r="T41" s="70">
-        <f>SUM(P41:S41)</f>
-        <v>150000</v>
-      </c>
-      <c r="U41" s="68">
-        <f>VLOOKUP(P39,$C$25:$G$37,2,0)</f>
-        <v>150000</v>
-      </c>
-    </row>
-    <row r="42" spans="3:22" x14ac:dyDescent="0.2">
+      <c r="S41" s="80">
+        <f>S29-O40</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="3:19" x14ac:dyDescent="0.2">
       <c r="F42"/>
       <c r="G42"/>
-      <c r="O42" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="P42" s="21">
-        <v>0</v>
-      </c>
-      <c r="Q42" s="21">
-        <v>0</v>
-      </c>
-      <c r="R42" s="21">
-        <v>0</v>
-      </c>
-      <c r="S42" s="64">
-        <v>0</v>
-      </c>
-      <c r="T42" s="43">
-        <f t="shared" ref="T42:T44" si="6">SUM(P42:S42)</f>
-        <v>0</v>
-      </c>
-      <c r="U42" s="68">
-        <f>VLOOKUP(P39,$C$25:$G$37,3,0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="3:22" x14ac:dyDescent="0.2">
+      <c r="N42" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="O42" s="30">
+        <v>0</v>
+      </c>
+      <c r="P42" s="30">
+        <v>0</v>
+      </c>
+      <c r="Q42" s="30">
+        <v>0</v>
+      </c>
+      <c r="R42" s="67">
+        <v>0</v>
+      </c>
+      <c r="S42" s="71">
+        <f>SUM(O42:R42)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="3:19" x14ac:dyDescent="0.2">
       <c r="F43"/>
       <c r="G43"/>
-      <c r="O43" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="P43" s="21">
-        <v>0</v>
-      </c>
-      <c r="Q43" s="21">
-        <v>110000</v>
-      </c>
-      <c r="R43" s="21">
-        <v>0</v>
-      </c>
-      <c r="S43" s="64">
-        <v>0</v>
-      </c>
-      <c r="T43" s="43">
-        <f t="shared" si="6"/>
-        <v>110000</v>
-      </c>
-      <c r="U43" s="68">
-        <f>VLOOKUP(P39,$C$25:$G$37,4,0)</f>
-        <v>110000</v>
-      </c>
-      <c r="V43" s="16" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="44" spans="3:22" x14ac:dyDescent="0.2">
+      <c r="S43" s="81">
+        <f>SUMPRODUCT($D$23:$G$23,O42:R42)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="3:19" x14ac:dyDescent="0.2">
       <c r="F44"/>
       <c r="G44"/>
-      <c r="O44" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="P44" s="60">
-        <v>0</v>
-      </c>
-      <c r="Q44" s="60">
-        <v>0</v>
-      </c>
-      <c r="R44" s="60">
-        <v>0</v>
-      </c>
-      <c r="S44" s="65">
-        <v>0</v>
-      </c>
-      <c r="T44" s="44">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="U44" s="69">
-        <f>VLOOKUP(P39,$C$25:$G$37,5,0)</f>
-        <v>0</v>
-      </c>
-      <c r="V44" s="71">
-        <f>SUMPRODUCT($D$8:$G$11,P41:S44)</f>
-        <v>2178400</v>
-      </c>
-    </row>
-    <row r="45" spans="3:22" x14ac:dyDescent="0.2">
+    </row>
+    <row r="45" spans="3:19" x14ac:dyDescent="0.2">
       <c r="F45"/>
       <c r="G45"/>
     </row>
-    <row r="46" spans="3:22" x14ac:dyDescent="0.2">
+    <row r="46" spans="3:19" x14ac:dyDescent="0.2">
       <c r="F46"/>
       <c r="G46"/>
-      <c r="O46" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="P46" s="32">
-        <v>1500000</v>
-      </c>
-      <c r="Q46" s="32">
-        <v>750000</v>
-      </c>
-      <c r="R46" s="32">
-        <v>1250000</v>
-      </c>
-      <c r="S46" s="33">
-        <v>1000000</v>
-      </c>
-      <c r="V46" s="16" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="47" spans="3:22" x14ac:dyDescent="0.2">
-      <c r="O47" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="P47" s="13">
-        <f>P27+SUM(P20:P23)+SUM(P41:P44)</f>
-        <v>24000</v>
-      </c>
-      <c r="Q47" s="13">
-        <f t="shared" ref="Q47:S47" si="7">Q27+SUM(Q20:Q23)+SUM(Q41:Q44)</f>
-        <v>180000</v>
-      </c>
-      <c r="R47" s="13">
-        <f>R27+SUM(R20:R23)+SUM(R41:R44)</f>
-        <v>160000</v>
-      </c>
-      <c r="S47" s="14">
-        <f t="shared" si="7"/>
-        <v>136000</v>
-      </c>
-      <c r="V47" s="71">
-        <f>SUMPRODUCT($D$19:$G$19,P47:S47)</f>
-        <v>3440800</v>
-      </c>
-    </row>
-    <row r="49" spans="15:22" x14ac:dyDescent="0.2">
-      <c r="O49" s="46" t="s">
-        <v>25</v>
-      </c>
-      <c r="P49" s="32">
-        <v>24000</v>
-      </c>
-      <c r="Q49" s="32">
-        <v>180000</v>
-      </c>
-      <c r="R49" s="32">
-        <v>160000</v>
-      </c>
-      <c r="S49" s="33">
-        <v>170000</v>
-      </c>
-      <c r="V49" s="16" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="50" spans="15:22" x14ac:dyDescent="0.2">
-      <c r="O50" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="P50" s="30">
-        <v>24000</v>
-      </c>
-      <c r="Q50" s="30">
-        <v>180000</v>
-      </c>
-      <c r="R50" s="30">
-        <v>160000</v>
-      </c>
-      <c r="S50" s="67">
-        <v>136000</v>
-      </c>
-      <c r="V50" s="71">
-        <f>SUMPRODUCT($D$21:$G$21,P50:S50)</f>
-        <v>5459200</v>
-      </c>
-    </row>
-    <row r="52" spans="15:22" x14ac:dyDescent="0.2">
-      <c r="O52" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="P52" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q52" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="R52" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="S52" s="18" t="s">
-        <v>3</v>
-      </c>
-      <c r="T52" s="16" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="53" spans="15:22" x14ac:dyDescent="0.2">
-      <c r="O53" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="P53" s="21">
-        <v>0</v>
-      </c>
-      <c r="Q53" s="21">
-        <v>0</v>
-      </c>
-      <c r="R53" s="21">
-        <v>0</v>
-      </c>
-      <c r="S53" s="64">
-        <v>0</v>
-      </c>
-      <c r="T53" s="43">
-        <f>SUM(P53:S53)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="15:22" x14ac:dyDescent="0.2">
-      <c r="O54" s="19" t="s">
-        <v>1</v>
-      </c>
-      <c r="P54" s="21">
-        <v>0</v>
-      </c>
-      <c r="Q54" s="21">
-        <v>0</v>
-      </c>
-      <c r="R54" s="21">
-        <v>0</v>
-      </c>
-      <c r="S54" s="64">
-        <v>0</v>
-      </c>
-      <c r="T54" s="43">
-        <f t="shared" ref="T54:T56" si="8">SUM(P54:S54)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="15:22" x14ac:dyDescent="0.2">
-      <c r="O55" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="P55" s="21">
-        <v>0</v>
-      </c>
-      <c r="Q55" s="21">
-        <v>0</v>
-      </c>
-      <c r="R55" s="21">
-        <v>0</v>
-      </c>
-      <c r="S55" s="64">
-        <v>0</v>
-      </c>
-      <c r="T55" s="43">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="V55" s="16" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="56" spans="15:22" x14ac:dyDescent="0.2">
-      <c r="O56" s="20" t="s">
-        <v>3</v>
-      </c>
-      <c r="P56" s="60">
-        <v>0</v>
-      </c>
-      <c r="Q56" s="60">
-        <v>0</v>
-      </c>
-      <c r="R56" s="60">
-        <v>0</v>
-      </c>
-      <c r="S56" s="65">
-        <v>0</v>
-      </c>
-      <c r="T56" s="44">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="V56" s="71">
-        <f>SUMPRODUCT($D$14:$G$17,P53:S56)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="15:22" x14ac:dyDescent="0.2">
-      <c r="O58" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="P58" s="13">
-        <f>T53</f>
-        <v>0</v>
-      </c>
-      <c r="Q58" s="13">
-        <f>T54</f>
-        <v>0</v>
-      </c>
-      <c r="R58" s="13">
-        <f>T55</f>
-        <v>0</v>
-      </c>
-      <c r="S58" s="14">
-        <f>T56</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" spans="15:22" x14ac:dyDescent="0.2">
-      <c r="O60" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="P60" s="13">
-        <f>P47-P50-P58</f>
-        <v>0</v>
-      </c>
-      <c r="Q60" s="13">
-        <f>Q47-Q50-Q58</f>
-        <v>0</v>
-      </c>
-      <c r="R60" s="13">
-        <f>R47-R50-R58</f>
-        <v>0</v>
-      </c>
-      <c r="S60" s="14">
-        <f>S47-S50-S58</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="62" spans="15:22" x14ac:dyDescent="0.2">
-      <c r="O62" s="46" t="s">
-        <v>61</v>
-      </c>
-      <c r="P62" s="32">
-        <v>1000000</v>
-      </c>
-      <c r="Q62" s="32">
-        <v>800000</v>
-      </c>
-      <c r="R62" s="32">
-        <v>1000000</v>
-      </c>
-      <c r="S62" s="33">
-        <v>900000</v>
-      </c>
-      <c r="V62" s="16" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="63" spans="15:22" x14ac:dyDescent="0.2">
-      <c r="O63" s="16" t="s">
-        <v>53</v>
-      </c>
-      <c r="P63" s="13">
-        <f>P35+P50</f>
-        <v>24000</v>
-      </c>
-      <c r="Q63" s="13">
-        <f t="shared" ref="Q63:S63" si="9">Q35+Q50</f>
-        <v>180000</v>
-      </c>
-      <c r="R63" s="13">
-        <f t="shared" si="9"/>
-        <v>160000</v>
-      </c>
-      <c r="S63" s="14">
-        <f t="shared" si="9"/>
-        <v>136000</v>
-      </c>
-      <c r="V63" s="71">
-        <f>SUMPRODUCT($D$23:$G$23,P63:S63)</f>
-        <v>2118000</v>
-      </c>
-    </row>
-    <row r="65" spans="15:19" x14ac:dyDescent="0.2">
-      <c r="O65" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="P65" s="71">
-        <f>SUM(P63:S63)</f>
-        <v>500000</v>
-      </c>
-      <c r="Q65" s="16" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="66" spans="15:19" x14ac:dyDescent="0.2">
-      <c r="O66" s="16" t="s">
-        <v>54</v>
-      </c>
-      <c r="P66" s="72">
-        <v>500000</v>
-      </c>
-      <c r="Q66" s="71">
-        <f>P65-P66</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="68" spans="15:19" x14ac:dyDescent="0.2">
-      <c r="O68" s="16" t="s">
-        <v>59</v>
-      </c>
-      <c r="P68" s="30">
-        <v>0</v>
-      </c>
-      <c r="Q68" s="30">
-        <v>0</v>
-      </c>
-      <c r="R68" s="30">
-        <v>0</v>
-      </c>
-      <c r="S68" s="67">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="69" spans="15:19" x14ac:dyDescent="0.2">
-      <c r="O69" s="16" t="s">
-        <v>64</v>
-      </c>
-      <c r="P69" s="71">
-        <f>SUM(P68:S68)</f>
-        <v>0</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3954,12 +3568,12 @@
   <sheetData>
     <row r="17" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H17" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
     </row>
     <row r="20" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H20" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -3979,7 +3593,7 @@
   <sheetData>
     <row r="20" spans="7:12" x14ac:dyDescent="0.2">
       <c r="G20" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="H20">
         <v>12</v>
@@ -4003,7 +3617,7 @@
     </row>
     <row r="21" spans="7:12" x14ac:dyDescent="0.2">
       <c r="G21" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="H21">
         <v>45</v>
@@ -4027,7 +3641,7 @@
     </row>
     <row r="22" spans="7:12" x14ac:dyDescent="0.2">
       <c r="G22" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="H22">
         <v>17</v>
@@ -4051,7 +3665,7 @@
     </row>
     <row r="23" spans="7:12" x14ac:dyDescent="0.2">
       <c r="G23" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="H23">
         <v>29</v>
@@ -4075,7 +3689,7 @@
     </row>
     <row r="26" spans="7:12" x14ac:dyDescent="0.2">
       <c r="G26" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="H26">
         <v>65</v>
@@ -4083,7 +3697,7 @@
     </row>
     <row r="27" spans="7:12" x14ac:dyDescent="0.2">
       <c r="G27" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="H27">
         <f>SUM(H20:H23)-H26</f>

</xml_diff>